<commit_message>
Very basic first version of the HTML renderer
</commit_message>
<xml_diff>
--- a/rcc-ministry-catalog/src/main/resources/RCC Ministry Catalog.xlsx
+++ b/rcc-ministry-catalog/src/main/resources/RCC Ministry Catalog.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13020" yWindow="0" windowWidth="7860" windowHeight="8565"/>
+    <workbookView xWindow="16740" yWindow="0" windowWidth="7860" windowHeight="8565" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Outline" sheetId="5" r:id="rId1"/>
-    <sheet name="Audio Technician" sheetId="3" r:id="rId2"/>
-    <sheet name="Reference" sheetId="2" state="hidden" r:id="rId3"/>
+    <sheet name="Directory" sheetId="6" r:id="rId2"/>
+    <sheet name="Dictionary" sheetId="7" r:id="rId3"/>
+    <sheet name="Audio Technician" sheetId="3" r:id="rId4"/>
+    <sheet name="Reference" sheetId="2" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="GiftList">Lookups[Gifts]</definedName>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="233">
   <si>
     <t>Ministry Role:</t>
   </si>
@@ -282,9 +284,6 @@
     <t>Scott Knight</t>
   </si>
   <si>
-    <t>Head/POC</t>
-  </si>
-  <si>
     <t>Katy Hood</t>
   </si>
   <si>
@@ -426,9 +425,6 @@
     <t>Bob Booth</t>
   </si>
   <si>
-    <t>Lisa Murray, Bob Booth</t>
-  </si>
-  <si>
     <t>Todd Harrell</t>
   </si>
   <si>
@@ -474,9 +470,6 @@
     <t>High School</t>
   </si>
   <si>
-    <t>Jerry King, Katy Hood</t>
-  </si>
-  <si>
     <t>3.3.1</t>
   </si>
   <si>
@@ -552,9 +545,6 @@
     <t>Worship Team</t>
   </si>
   <si>
-    <t>Barbara Greb, Leigh Ann Skipper, John Dimeo</t>
-  </si>
-  <si>
     <t>5.1.1</t>
   </si>
   <si>
@@ -667,6 +657,81 @@
   </si>
   <si>
     <t>Prayer Retreats</t>
+  </si>
+  <si>
+    <t>Head/POC 1</t>
+  </si>
+  <si>
+    <t>Head/POC 2</t>
+  </si>
+  <si>
+    <t>Lisa Murray</t>
+  </si>
+  <si>
+    <t>Jerry King</t>
+  </si>
+  <si>
+    <t>Leigh Ann Skipper</t>
+  </si>
+  <si>
+    <t>John Dimeo</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>j.a.dimeo@gmail.com</t>
+  </si>
+  <si>
+    <t>434-964-0325</t>
+  </si>
+  <si>
+    <t>2bgreb@gmail.com</t>
+  </si>
+  <si>
+    <t>laskippy23@gmail.com</t>
+  </si>
+  <si>
+    <t>sknightrivanna@gmail.com</t>
+  </si>
+  <si>
+    <t>rivannachurch@gmail.com</t>
+  </si>
+  <si>
+    <t>434-975-0011</t>
+  </si>
+  <si>
+    <t>hoodgang0@gmail.com</t>
+  </si>
+  <si>
+    <t>tomstarkey01@gmail.com</t>
+  </si>
+  <si>
+    <t>elder.beth@gmail.com</t>
+  </si>
+  <si>
+    <t>rll9e@virginia.edu</t>
+  </si>
+  <si>
+    <t>harrelltm@yahoo.com</t>
+  </si>
+  <si>
+    <t>lamkem@yahoo.com</t>
+  </si>
+  <si>
+    <t>bboothjr93@gmail.com</t>
+  </si>
+  <si>
+    <t>Head/POC 3</t>
+  </si>
+  <si>
+    <t>Ministry Types</t>
   </si>
 </sst>
 </file>
@@ -791,7 +856,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -831,6 +896,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -864,9 +939,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -935,6 +1007,31 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TDirectory" displayName="TDirectory" ref="A1:C13" totalsRowShown="0">
+  <autoFilter ref="A1:C13"/>
+  <sortState ref="A2:C13">
+    <sortCondition ref="A1:A13"/>
+  </sortState>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Name"/>
+    <tableColumn id="2" name="Email" dataCellStyle="Hyperlink"/>
+    <tableColumn id="3" name="Phone"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TMinistryTypes" displayName="TMinistryTypes" ref="A1:A3" totalsRowShown="0">
+  <autoFilter ref="A1:A3"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Ministry Types"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Lookups" displayName="Lookups" ref="F1:H31" totalsRowShown="0">
   <autoFilter ref="F1:H31"/>
   <sortState ref="F2:G31">
@@ -1212,63 +1309,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G79"/>
+  <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1048576"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="8.7109375" style="30" customWidth="1"/>
+    <col min="1" max="3" width="8.7109375" style="17" customWidth="1"/>
     <col min="4" max="4" width="30.7109375" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" customWidth="1"/>
     <col min="7" max="7" width="20.7109375" style="16" customWidth="1"/>
+    <col min="8" max="9" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="30">
+      <c r="G1" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="17">
         <v>1</v>
       </c>
       <c r="D2" t="s">
         <v>74</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F2" t="s">
         <v>82</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="30">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="17">
         <v>1.1000000000000001</v>
       </c>
       <c r="D3" t="s">
@@ -1278,699 +1384,896 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C4" s="30" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C4" s="17" t="s">
         <v>76</v>
       </c>
       <c r="D4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C5" s="30" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C5" s="17" t="s">
         <v>79</v>
       </c>
       <c r="D5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="30">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="17">
         <v>1.2</v>
       </c>
       <c r="D6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C7" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" t="s">
         <v>85</v>
       </c>
-      <c r="G6" s="16" t="s">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C8" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C9" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="D10" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="D7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C8" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="D8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C9" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="D9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="30">
-        <v>1.3</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="G10" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="G10" s="16" t="s">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C11" s="17" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="30" t="s">
+      <c r="D11" t="s">
         <v>95</v>
       </c>
-      <c r="D11" t="s">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="17" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C12" s="30" t="s">
+      <c r="D12" t="s">
         <v>97</v>
       </c>
-      <c r="D12" t="s">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="17">
+        <v>1.4</v>
+      </c>
+      <c r="D13" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="30">
-        <v>1.4</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="G13" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="G13" s="16" t="s">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C14" s="17" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C14" s="30" t="s">
+      <c r="D14" t="s">
         <v>101</v>
       </c>
-      <c r="D14" t="s">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="D15" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="30">
-        <v>1.5</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="G15" s="16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="17">
+        <v>1.6</v>
+      </c>
+      <c r="D16" t="s">
         <v>103</v>
       </c>
-      <c r="G15" s="16" t="s">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="17">
+        <v>1.7</v>
+      </c>
+      <c r="D17" t="s">
+        <v>198</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="17">
+        <v>1.8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>199</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="17">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>104</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="H19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="17">
+        <v>2.1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C21" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="D21" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C22" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="D22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C23" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C24" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="D24" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="17">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D25" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C26" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="D26" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C27" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="D27" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C28" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="D28" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C29" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="D29" t="s">
+        <v>194</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C30" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D30" t="s">
+        <v>197</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="17">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D31" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C32" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="D32" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C33" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="D33" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C34" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="D34" t="s">
+        <v>202</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="17">
+        <v>2.4</v>
+      </c>
+      <c r="D35" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="17">
+        <v>3</v>
+      </c>
+      <c r="D36" t="s">
+        <v>126</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="17">
+        <v>3.1</v>
+      </c>
+      <c r="D37" t="s">
+        <v>128</v>
+      </c>
+      <c r="G37" s="16" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="30">
-        <v>1.6</v>
-      </c>
-      <c r="D16" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="30">
-        <v>1.7</v>
-      </c>
-      <c r="D17" t="s">
-        <v>202</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="30">
-        <v>1.8</v>
-      </c>
-      <c r="D18" t="s">
-        <v>203</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="30">
-        <v>2</v>
-      </c>
-      <c r="D19" t="s">
-        <v>105</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="G19" s="16" t="s">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="17">
+        <v>3.2</v>
+      </c>
+      <c r="D38" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="30">
-        <v>2.1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="D21" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="30" t="s">
-        <v>109</v>
-      </c>
-      <c r="D22" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="30" t="s">
-        <v>111</v>
-      </c>
-      <c r="D23" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="30" t="s">
-        <v>113</v>
-      </c>
-      <c r="D24" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="30">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="D25" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="30" t="s">
-        <v>116</v>
-      </c>
-      <c r="D26" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="D27" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="D28" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C29" s="30" t="s">
-        <v>197</v>
-      </c>
-      <c r="D29" t="s">
-        <v>198</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="30" t="s">
-        <v>200</v>
-      </c>
-      <c r="D30" t="s">
-        <v>201</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="30">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="D31" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C32" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="D32" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C33" s="30" t="s">
-        <v>124</v>
-      </c>
-      <c r="D33" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C34" s="30" t="s">
-        <v>204</v>
-      </c>
-      <c r="D34" t="s">
-        <v>206</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="30">
-        <v>2.4</v>
-      </c>
-      <c r="D35" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="30">
-        <v>3</v>
-      </c>
-      <c r="D36" t="s">
-        <v>127</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="30">
-        <v>3.1</v>
-      </c>
-      <c r="D37" t="s">
-        <v>129</v>
-      </c>
-      <c r="G37" s="16" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C39" s="17" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="30">
-        <v>3.2</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="D39" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C39" s="30" t="s">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C40" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C40" s="30" t="s">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C41" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D41" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C41" s="30" t="s">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C42" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D42" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C42" s="30" t="s">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C43" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D43" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C43" s="30" t="s">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C44" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D44" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C44" s="30" t="s">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="17">
+        <v>3.3</v>
+      </c>
+      <c r="D45" t="s">
         <v>144</v>
       </c>
-      <c r="D44" t="s">
+      <c r="G45" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="H45" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C46" s="17" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="30">
-        <v>3.3</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="D46" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C47" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="G45" s="16" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C46" s="30" t="s">
+      <c r="D47" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B48" s="17">
+        <v>3.4</v>
+      </c>
+      <c r="D48" t="s">
         <v>148</v>
       </c>
-      <c r="D46" t="s">
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C49" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="D49" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C47" s="30" t="s">
-        <v>149</v>
-      </c>
-      <c r="D47" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="30">
-        <v>3.4</v>
-      </c>
-      <c r="D48" t="s">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C50" s="17" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C49" s="30" t="s">
+      <c r="D50" t="s">
         <v>152</v>
       </c>
-      <c r="D49" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C50" s="30" t="s">
-        <v>154</v>
-      </c>
-      <c r="D50" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="30">
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="17">
         <v>4</v>
       </c>
       <c r="D51" t="s">
         <v>71</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F51" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B52" s="17">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D52" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C53" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="D53" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B52" s="30">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="D52" t="s">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C54" s="17" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C53" s="30" t="s">
+      <c r="D54" t="s">
         <v>159</v>
       </c>
-      <c r="D53" t="s">
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C55" s="17" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C54" s="30" t="s">
+      <c r="D55" t="s">
         <v>161</v>
       </c>
-      <c r="D54" t="s">
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C56" s="17" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C55" s="30" t="s">
+      <c r="D56" t="s">
         <v>163</v>
       </c>
-      <c r="D55" t="s">
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B57" s="17">
+        <v>4.2</v>
+      </c>
+      <c r="D57" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C56" s="30" t="s">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C58" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D58" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B57" s="30">
-        <v>4.2</v>
-      </c>
-      <c r="D57" t="s">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C59" s="17" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C58" s="30" t="s">
+      <c r="D59" t="s">
         <v>168</v>
       </c>
-      <c r="D58" t="s">
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="17">
+        <v>5</v>
+      </c>
+      <c r="D60" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C59" s="30" t="s">
-        <v>170</v>
-      </c>
-      <c r="D59" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="30">
-        <v>5</v>
-      </c>
-      <c r="D60" t="s">
-        <v>172</v>
-      </c>
       <c r="E60" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F60" t="s">
         <v>82</v>
       </c>
       <c r="G60" s="16" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B61" s="30">
+        <v>205</v>
+      </c>
+      <c r="H60" t="s">
+        <v>212</v>
+      </c>
+      <c r="I60" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B61" s="17">
         <v>5.0999999999999996</v>
       </c>
       <c r="D61" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C62" s="30" t="s">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C62" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="D62" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C63" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="D63" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C64" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="D64" t="s">
+        <v>203</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G64" s="16" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B65" s="17">
+        <v>5.2</v>
+      </c>
+      <c r="D65" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C66" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D66" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C67" s="17" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C63" s="30" t="s">
+      <c r="D67" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C68" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="D63" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C64" s="30" t="s">
-        <v>208</v>
-      </c>
-      <c r="D64" t="s">
-        <v>207</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G64" s="16" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B65" s="30">
-        <v>5.2</v>
-      </c>
-      <c r="D65" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C66" s="30" t="s">
-        <v>178</v>
-      </c>
-      <c r="D66" t="s">
+      <c r="D68" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="17">
+        <v>6</v>
+      </c>
+      <c r="D69" t="s">
+        <v>188</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B70" s="17">
+        <v>6.1</v>
+      </c>
+      <c r="D70" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B71" s="17">
+        <v>6.2</v>
+      </c>
+      <c r="D71" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C72" s="17" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C67" s="30" t="s">
-        <v>179</v>
-      </c>
-      <c r="D67" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C68" s="30" t="s">
-        <v>180</v>
-      </c>
-      <c r="D68" t="s">
+      <c r="D72" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="30">
-        <v>6</v>
-      </c>
-      <c r="D69" t="s">
-        <v>192</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B70" s="30">
-        <v>6.1</v>
-      </c>
-      <c r="D70" t="s">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C73" s="17" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B71" s="30">
-        <v>6.2</v>
-      </c>
-      <c r="D71" t="s">
+      <c r="D73" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C72" s="30" t="s">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C74" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D74" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C73" s="30" t="s">
-        <v>188</v>
-      </c>
-      <c r="D73" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C74" s="30" t="s">
-        <v>190</v>
-      </c>
-      <c r="D74" t="s">
-        <v>191</v>
-      </c>
-    </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="30">
+      <c r="A75" s="17">
         <v>7</v>
       </c>
       <c r="D75" t="s">
         <v>32</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G75" s="16" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B76" s="30">
+      <c r="B76" s="17">
         <v>7.1</v>
       </c>
       <c r="D76" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B77" s="30">
+      <c r="B77" s="17">
         <v>7.2</v>
       </c>
       <c r="D77" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B78" s="17">
+        <v>7.3</v>
+      </c>
+      <c r="D78" t="s">
+        <v>206</v>
+      </c>
+      <c r="E78" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B78" s="30">
-        <v>7.3</v>
-      </c>
-      <c r="D78" t="s">
-        <v>210</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B79" s="30">
+      <c r="B79" s="17">
         <v>7.4</v>
       </c>
       <c r="D79" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Not in directory" error="You have entered a person who is not in the Directory tab" sqref="G2:I200">
+      <formula1>INDIRECT("TDirectory[Name]")</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E220">
+      <formula1>INDIRECT("TMinistryTypes[Ministry Types]")</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" t="s">
+        <v>222</v>
+      </c>
+      <c r="C5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="C7" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>212</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>210</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>154</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>225</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B9" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E85"/>
   <sheetViews>
@@ -1992,10 +2295,10 @@
         <f>Reference!A1</f>
         <v>Ministry Role:</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="19"/>
+      <c r="D1" s="23"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2012,10 +2315,10 @@
         <f>Reference!A3</f>
         <v>Filled by:</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="21"/>
+      <c r="D3" s="25"/>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2026,11 +2329,11 @@
         <f>Reference!A5</f>
         <v>In Ministry Area:</v>
       </c>
-      <c r="C5" s="22" t="e">
+      <c r="C5" s="26" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="D5" s="22"/>
+      <c r="D5" s="26"/>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2038,11 +2341,11 @@
         <f>Reference!A6</f>
         <v>Under Ministry Role:</v>
       </c>
-      <c r="C6" s="22" t="e">
+      <c r="C6" s="26" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="D6" s="22"/>
+      <c r="D6" s="26"/>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2073,10 +2376,10 @@
         <f>Reference!A10</f>
         <v>Position open to:</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="D10" s="21"/>
+      <c r="D10" s="25"/>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" ht="8.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2085,31 +2388,31 @@
         <f>Reference!A12</f>
         <v>Relevant gifts:</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="18"/>
+      <c r="D12" s="22"/>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="18"/>
+      <c r="D13" s="22"/>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="18"/>
+      <c r="D14" s="22"/>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="18"/>
+      <c r="D15" s="22"/>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2123,32 +2426,32 @@
         <f>Reference!A19</f>
         <v>Relevant skills:</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="18"/>
+      <c r="D17" s="22"/>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="18"/>
+      <c r="D18" s="22"/>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="D19" s="18"/>
+      <c r="D19" s="22"/>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D20" s="18"/>
+      <c r="D20" s="22"/>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2162,24 +2465,24 @@
         <f>Reference!A25</f>
         <v>Personality:</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="D22" s="18"/>
+      <c r="D22" s="22"/>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="18"/>
+      <c r="D23" s="22"/>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="D24" s="18"/>
+      <c r="D24" s="22"/>
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2192,10 +2495,10 @@
         <f>Reference!A31</f>
         <v>Length of service:</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="D26" s="18"/>
+      <c r="D26" s="22"/>
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -2203,17 +2506,17 @@
         <f>Reference!A32</f>
         <v>Time commitments:</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="D27" s="18"/>
+      <c r="D27" s="22"/>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="18"/>
+      <c r="D28" s="22"/>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2226,243 +2529,243 @@
         <f>Reference!A38</f>
         <v>Responsibilities:</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="C30" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="D30" s="18"/>
+      <c r="D30" s="22"/>
       <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C31" s="17" t="s">
+      <c r="C31" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="D31" s="18"/>
+      <c r="D31" s="22"/>
       <c r="E31" s="5"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C32" s="17" t="s">
+      <c r="C32" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="D32" s="18"/>
+      <c r="D32" s="22"/>
       <c r="E32" s="5"/>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C33" s="17" t="s">
+      <c r="C33" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="D33" s="18"/>
+      <c r="D33" s="22"/>
       <c r="E33" s="5"/>
     </row>
     <row r="34" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C34" s="17" t="s">
+      <c r="C34" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="D34" s="18"/>
+      <c r="D34" s="22"/>
       <c r="E34" s="5"/>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
     </row>
     <row r="36" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C36" s="23"/>
-      <c r="D36" s="23"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C37" s="23"/>
-      <c r="D37" s="23"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C38" s="23"/>
-      <c r="D38" s="23"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C39" s="23"/>
-      <c r="D39" s="23"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
     </row>
     <row r="40" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C40" s="23"/>
-      <c r="D40" s="23"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C41" s="23"/>
-      <c r="D41" s="23"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27"/>
     </row>
     <row r="42" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C42" s="23"/>
-      <c r="D42" s="23"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="27"/>
     </row>
     <row r="43" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C43" s="23"/>
-      <c r="D43" s="23"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
     </row>
     <row r="44" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C44" s="23"/>
-      <c r="D44" s="23"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27"/>
     </row>
     <row r="45" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C45" s="23"/>
-      <c r="D45" s="23"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="27"/>
     </row>
     <row r="46" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C46" s="23"/>
-      <c r="D46" s="23"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="27"/>
     </row>
     <row r="47" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C47" s="23"/>
-      <c r="D47" s="23"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
     </row>
     <row r="48" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C48" s="23"/>
-      <c r="D48" s="23"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="27"/>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C49" s="23"/>
-      <c r="D49" s="23"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="27"/>
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C50" s="23"/>
-      <c r="D50" s="23"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="27"/>
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C51" s="23"/>
-      <c r="D51" s="23"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="27"/>
     </row>
     <row r="52" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C52" s="23"/>
-      <c r="D52" s="23"/>
+      <c r="C52" s="27"/>
+      <c r="D52" s="27"/>
     </row>
     <row r="53" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C53" s="23"/>
-      <c r="D53" s="23"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="27"/>
     </row>
     <row r="54" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C54" s="23"/>
-      <c r="D54" s="23"/>
+      <c r="C54" s="27"/>
+      <c r="D54" s="27"/>
     </row>
     <row r="55" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C55" s="23"/>
-      <c r="D55" s="23"/>
+      <c r="C55" s="27"/>
+      <c r="D55" s="27"/>
     </row>
     <row r="56" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C56" s="23"/>
-      <c r="D56" s="23"/>
+      <c r="C56" s="27"/>
+      <c r="D56" s="27"/>
     </row>
     <row r="57" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C57" s="23"/>
-      <c r="D57" s="23"/>
+      <c r="C57" s="27"/>
+      <c r="D57" s="27"/>
     </row>
     <row r="58" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C58" s="23"/>
-      <c r="D58" s="23"/>
+      <c r="C58" s="27"/>
+      <c r="D58" s="27"/>
     </row>
     <row r="59" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C59" s="23"/>
-      <c r="D59" s="23"/>
+      <c r="C59" s="27"/>
+      <c r="D59" s="27"/>
     </row>
     <row r="60" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C60" s="23"/>
-      <c r="D60" s="23"/>
+      <c r="C60" s="27"/>
+      <c r="D60" s="27"/>
     </row>
     <row r="61" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C61" s="23"/>
-      <c r="D61" s="23"/>
+      <c r="C61" s="27"/>
+      <c r="D61" s="27"/>
     </row>
     <row r="62" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C62" s="23"/>
-      <c r="D62" s="23"/>
+      <c r="C62" s="27"/>
+      <c r="D62" s="27"/>
     </row>
     <row r="63" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C63" s="23"/>
-      <c r="D63" s="23"/>
+      <c r="C63" s="27"/>
+      <c r="D63" s="27"/>
     </row>
     <row r="64" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C64" s="23"/>
-      <c r="D64" s="23"/>
+      <c r="C64" s="27"/>
+      <c r="D64" s="27"/>
     </row>
     <row r="65" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C65" s="23"/>
-      <c r="D65" s="23"/>
+      <c r="C65" s="27"/>
+      <c r="D65" s="27"/>
     </row>
     <row r="66" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C66" s="23"/>
-      <c r="D66" s="23"/>
+      <c r="C66" s="27"/>
+      <c r="D66" s="27"/>
     </row>
     <row r="67" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C67" s="23"/>
-      <c r="D67" s="23"/>
+      <c r="C67" s="27"/>
+      <c r="D67" s="27"/>
     </row>
     <row r="68" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C68" s="23"/>
-      <c r="D68" s="23"/>
+      <c r="C68" s="27"/>
+      <c r="D68" s="27"/>
     </row>
     <row r="69" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C69" s="23"/>
-      <c r="D69" s="23"/>
+      <c r="C69" s="27"/>
+      <c r="D69" s="27"/>
     </row>
     <row r="70" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C70" s="23"/>
-      <c r="D70" s="23"/>
+      <c r="C70" s="27"/>
+      <c r="D70" s="27"/>
     </row>
     <row r="71" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C71" s="23"/>
-      <c r="D71" s="23"/>
+      <c r="C71" s="27"/>
+      <c r="D71" s="27"/>
     </row>
     <row r="72" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C72" s="23"/>
-      <c r="D72" s="23"/>
+      <c r="C72" s="27"/>
+      <c r="D72" s="27"/>
     </row>
     <row r="73" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C73" s="23"/>
-      <c r="D73" s="23"/>
+      <c r="C73" s="27"/>
+      <c r="D73" s="27"/>
     </row>
     <row r="74" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C74" s="23"/>
-      <c r="D74" s="23"/>
+      <c r="C74" s="27"/>
+      <c r="D74" s="27"/>
     </row>
     <row r="75" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C75" s="23"/>
-      <c r="D75" s="23"/>
+      <c r="C75" s="27"/>
+      <c r="D75" s="27"/>
     </row>
     <row r="76" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C76" s="23"/>
-      <c r="D76" s="23"/>
+      <c r="C76" s="27"/>
+      <c r="D76" s="27"/>
     </row>
     <row r="77" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C77" s="23"/>
-      <c r="D77" s="23"/>
+      <c r="C77" s="27"/>
+      <c r="D77" s="27"/>
     </row>
     <row r="78" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C78" s="23"/>
-      <c r="D78" s="23"/>
+      <c r="C78" s="27"/>
+      <c r="D78" s="27"/>
     </row>
     <row r="79" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C79" s="23"/>
-      <c r="D79" s="23"/>
+      <c r="C79" s="27"/>
+      <c r="D79" s="27"/>
     </row>
     <row r="80" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C80" s="23"/>
-      <c r="D80" s="23"/>
+      <c r="C80" s="27"/>
+      <c r="D80" s="27"/>
     </row>
     <row r="81" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C81" s="23"/>
-      <c r="D81" s="23"/>
+      <c r="C81" s="27"/>
+      <c r="D81" s="27"/>
     </row>
     <row r="82" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C82" s="23"/>
-      <c r="D82" s="23"/>
+      <c r="C82" s="27"/>
+      <c r="D82" s="27"/>
     </row>
     <row r="83" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C83" s="23"/>
-      <c r="D83" s="23"/>
+      <c r="C83" s="27"/>
+      <c r="D83" s="27"/>
     </row>
     <row r="84" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C84" s="23"/>
-      <c r="D84" s="23"/>
+      <c r="C84" s="27"/>
+      <c r="D84" s="27"/>
     </row>
     <row r="85" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C85" s="23"/>
-      <c r="D85" s="23"/>
+      <c r="C85" s="27"/>
+      <c r="D85" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="75">
@@ -2576,7 +2879,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H95"/>
   <sheetViews>
@@ -2600,8 +2903,8 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
       <c r="E1" s="1"/>
       <c r="F1" t="s">
         <v>45</v>
@@ -2634,8 +2937,8 @@
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="25"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="29"/>
       <c r="E3" s="2"/>
       <c r="F3" t="s">
         <v>2</v>
@@ -2660,8 +2963,8 @@
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
       <c r="E5" s="2"/>
       <c r="G5" t="s">
         <v>29</v>
@@ -2671,8 +2974,8 @@
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
       <c r="E6" s="2"/>
       <c r="G6" t="s">
         <v>23</v>
@@ -2710,8 +3013,8 @@
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="25"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="29"/>
       <c r="E10" s="2"/>
       <c r="G10" t="s">
         <v>22</v>
@@ -2727,8 +3030,8 @@
       <c r="A12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="25"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="29"/>
       <c r="E12" s="2"/>
       <c r="G12" t="s">
         <v>30</v>
@@ -2736,8 +3039,8 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="25"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="29"/>
       <c r="E13" s="2"/>
       <c r="G13" t="s">
         <v>31</v>
@@ -2745,8 +3048,8 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="25"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="29"/>
       <c r="E14" s="2"/>
       <c r="G14" t="s">
         <v>33</v>
@@ -2754,8 +3057,8 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="25"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="29"/>
       <c r="E15" s="2"/>
       <c r="G15" t="s">
         <v>34</v>
@@ -2763,8 +3066,8 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="25"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="29"/>
       <c r="E16" s="2"/>
       <c r="G16" t="s">
         <v>35</v>
@@ -2792,8 +3095,8 @@
       <c r="A19" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="25"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="29"/>
       <c r="E19" s="2"/>
       <c r="G19" t="s">
         <v>16</v>
@@ -2801,8 +3104,8 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="25"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="29"/>
       <c r="E20" s="2"/>
       <c r="G20" t="s">
         <v>43</v>
@@ -2810,8 +3113,8 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="25"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="29"/>
       <c r="E21" s="2"/>
       <c r="G21" t="s">
         <v>15</v>
@@ -2819,8 +3122,8 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="25"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="29"/>
       <c r="E22" s="2"/>
       <c r="G22" t="s">
         <v>32</v>
@@ -2828,8 +3131,8 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="25"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="29"/>
       <c r="E23" s="2"/>
       <c r="G23" t="s">
         <v>41</v>
@@ -2848,8 +3151,8 @@
       <c r="A25" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C25" s="24"/>
-      <c r="D25" s="25"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="29"/>
       <c r="E25" s="2"/>
       <c r="G25" t="s">
         <v>40</v>
@@ -2857,8 +3160,8 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="25"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="29"/>
       <c r="E26" s="2"/>
       <c r="G26" t="s">
         <v>17</v>
@@ -2866,8 +3169,8 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="25"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="29"/>
       <c r="E27" s="2"/>
       <c r="G27" t="s">
         <v>36</v>
@@ -2875,8 +3178,8 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="25"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="29"/>
       <c r="E28" s="2"/>
       <c r="G28" t="s">
         <v>25</v>
@@ -2884,8 +3187,8 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="25"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="29"/>
       <c r="E29" s="2"/>
       <c r="G29" t="s">
         <v>26</v>
@@ -2904,8 +3207,8 @@
       <c r="A31" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C31" s="24"/>
-      <c r="D31" s="25"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="29"/>
       <c r="E31" s="2"/>
       <c r="G31" t="s">
         <v>27</v>
@@ -2915,32 +3218,32 @@
       <c r="A32" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="24"/>
-      <c r="D32" s="25"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="29"/>
       <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="25"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="29"/>
       <c r="E33" s="2"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="25"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="29"/>
       <c r="E34" s="2"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="25"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="29"/>
       <c r="E35" s="2"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="25"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="29"/>
       <c r="E36" s="2"/>
     </row>
     <row r="37" spans="1:5" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2953,244 +3256,244 @@
       <c r="A38" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="24"/>
-      <c r="D38" s="25"/>
+      <c r="C38" s="28"/>
+      <c r="D38" s="29"/>
       <c r="E38" s="2"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="29"/>
+      <c r="C39" s="32"/>
+      <c r="D39" s="33"/>
       <c r="E39" s="5"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C40" s="28"/>
-      <c r="D40" s="29"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="33"/>
       <c r="E40" s="5"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C41" s="28"/>
-      <c r="D41" s="29"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="33"/>
       <c r="E41" s="5"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C42" s="28"/>
-      <c r="D42" s="29"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="33"/>
       <c r="E42" s="5"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C43" s="28"/>
-      <c r="D43" s="29"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="33"/>
       <c r="E43" s="5"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C44" s="28"/>
-      <c r="D44" s="29"/>
+      <c r="C44" s="32"/>
+      <c r="D44" s="33"/>
       <c r="E44" s="5"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C45" s="23"/>
-      <c r="D45" s="23"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="27"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C46" s="23"/>
-      <c r="D46" s="23"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="27"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C47" s="23"/>
-      <c r="D47" s="23"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C48" s="23"/>
-      <c r="D48" s="23"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="27"/>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C49" s="23"/>
-      <c r="D49" s="23"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="27"/>
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C50" s="23"/>
-      <c r="D50" s="23"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="27"/>
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C51" s="23"/>
-      <c r="D51" s="23"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="27"/>
     </row>
     <row r="52" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C52" s="23"/>
-      <c r="D52" s="23"/>
+      <c r="C52" s="27"/>
+      <c r="D52" s="27"/>
     </row>
     <row r="53" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C53" s="23"/>
-      <c r="D53" s="23"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="27"/>
     </row>
     <row r="54" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C54" s="23"/>
-      <c r="D54" s="23"/>
+      <c r="C54" s="27"/>
+      <c r="D54" s="27"/>
     </row>
     <row r="55" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C55" s="23"/>
-      <c r="D55" s="23"/>
+      <c r="C55" s="27"/>
+      <c r="D55" s="27"/>
     </row>
     <row r="56" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C56" s="23"/>
-      <c r="D56" s="23"/>
+      <c r="C56" s="27"/>
+      <c r="D56" s="27"/>
     </row>
     <row r="57" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C57" s="23"/>
-      <c r="D57" s="23"/>
+      <c r="C57" s="27"/>
+      <c r="D57" s="27"/>
     </row>
     <row r="58" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C58" s="23"/>
-      <c r="D58" s="23"/>
+      <c r="C58" s="27"/>
+      <c r="D58" s="27"/>
     </row>
     <row r="59" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C59" s="23"/>
-      <c r="D59" s="23"/>
+      <c r="C59" s="27"/>
+      <c r="D59" s="27"/>
     </row>
     <row r="60" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C60" s="23"/>
-      <c r="D60" s="23"/>
+      <c r="C60" s="27"/>
+      <c r="D60" s="27"/>
     </row>
     <row r="61" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C61" s="23"/>
-      <c r="D61" s="23"/>
+      <c r="C61" s="27"/>
+      <c r="D61" s="27"/>
     </row>
     <row r="62" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C62" s="23"/>
-      <c r="D62" s="23"/>
+      <c r="C62" s="27"/>
+      <c r="D62" s="27"/>
     </row>
     <row r="63" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C63" s="23"/>
-      <c r="D63" s="23"/>
+      <c r="C63" s="27"/>
+      <c r="D63" s="27"/>
     </row>
     <row r="64" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C64" s="23"/>
-      <c r="D64" s="23"/>
+      <c r="C64" s="27"/>
+      <c r="D64" s="27"/>
     </row>
     <row r="65" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C65" s="23"/>
-      <c r="D65" s="23"/>
+      <c r="C65" s="27"/>
+      <c r="D65" s="27"/>
     </row>
     <row r="66" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C66" s="23"/>
-      <c r="D66" s="23"/>
+      <c r="C66" s="27"/>
+      <c r="D66" s="27"/>
     </row>
     <row r="67" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C67" s="23"/>
-      <c r="D67" s="23"/>
+      <c r="C67" s="27"/>
+      <c r="D67" s="27"/>
     </row>
     <row r="68" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C68" s="23"/>
-      <c r="D68" s="23"/>
+      <c r="C68" s="27"/>
+      <c r="D68" s="27"/>
     </row>
     <row r="69" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C69" s="23"/>
-      <c r="D69" s="23"/>
+      <c r="C69" s="27"/>
+      <c r="D69" s="27"/>
     </row>
     <row r="70" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C70" s="23"/>
-      <c r="D70" s="23"/>
+      <c r="C70" s="27"/>
+      <c r="D70" s="27"/>
     </row>
     <row r="71" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C71" s="23"/>
-      <c r="D71" s="23"/>
+      <c r="C71" s="27"/>
+      <c r="D71" s="27"/>
     </row>
     <row r="72" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C72" s="23"/>
-      <c r="D72" s="23"/>
+      <c r="C72" s="27"/>
+      <c r="D72" s="27"/>
     </row>
     <row r="73" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C73" s="23"/>
-      <c r="D73" s="23"/>
+      <c r="C73" s="27"/>
+      <c r="D73" s="27"/>
     </row>
     <row r="74" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C74" s="23"/>
-      <c r="D74" s="23"/>
+      <c r="C74" s="27"/>
+      <c r="D74" s="27"/>
     </row>
     <row r="75" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C75" s="23"/>
-      <c r="D75" s="23"/>
+      <c r="C75" s="27"/>
+      <c r="D75" s="27"/>
     </row>
     <row r="76" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C76" s="23"/>
-      <c r="D76" s="23"/>
+      <c r="C76" s="27"/>
+      <c r="D76" s="27"/>
     </row>
     <row r="77" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C77" s="23"/>
-      <c r="D77" s="23"/>
+      <c r="C77" s="27"/>
+      <c r="D77" s="27"/>
     </row>
     <row r="78" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C78" s="23"/>
-      <c r="D78" s="23"/>
+      <c r="C78" s="27"/>
+      <c r="D78" s="27"/>
     </row>
     <row r="79" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C79" s="23"/>
-      <c r="D79" s="23"/>
+      <c r="C79" s="27"/>
+      <c r="D79" s="27"/>
     </row>
     <row r="80" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C80" s="23"/>
-      <c r="D80" s="23"/>
+      <c r="C80" s="27"/>
+      <c r="D80" s="27"/>
     </row>
     <row r="81" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C81" s="23"/>
-      <c r="D81" s="23"/>
+      <c r="C81" s="27"/>
+      <c r="D81" s="27"/>
     </row>
     <row r="82" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C82" s="23"/>
-      <c r="D82" s="23"/>
+      <c r="C82" s="27"/>
+      <c r="D82" s="27"/>
     </row>
     <row r="83" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C83" s="23"/>
-      <c r="D83" s="23"/>
+      <c r="C83" s="27"/>
+      <c r="D83" s="27"/>
     </row>
     <row r="84" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C84" s="23"/>
-      <c r="D84" s="23"/>
+      <c r="C84" s="27"/>
+      <c r="D84" s="27"/>
     </row>
     <row r="85" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C85" s="23"/>
-      <c r="D85" s="23"/>
+      <c r="C85" s="27"/>
+      <c r="D85" s="27"/>
     </row>
     <row r="86" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C86" s="23"/>
-      <c r="D86" s="23"/>
+      <c r="C86" s="27"/>
+      <c r="D86" s="27"/>
     </row>
     <row r="87" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C87" s="23"/>
-      <c r="D87" s="23"/>
+      <c r="C87" s="27"/>
+      <c r="D87" s="27"/>
     </row>
     <row r="88" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C88" s="23"/>
-      <c r="D88" s="23"/>
+      <c r="C88" s="27"/>
+      <c r="D88" s="27"/>
     </row>
     <row r="89" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C89" s="23"/>
-      <c r="D89" s="23"/>
+      <c r="C89" s="27"/>
+      <c r="D89" s="27"/>
     </row>
     <row r="90" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C90" s="23"/>
-      <c r="D90" s="23"/>
+      <c r="C90" s="27"/>
+      <c r="D90" s="27"/>
     </row>
     <row r="91" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C91" s="23"/>
-      <c r="D91" s="23"/>
+      <c r="C91" s="27"/>
+      <c r="D91" s="27"/>
     </row>
     <row r="92" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C92" s="23"/>
-      <c r="D92" s="23"/>
+      <c r="C92" s="27"/>
+      <c r="D92" s="27"/>
     </row>
     <row r="93" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C93" s="23"/>
-      <c r="D93" s="23"/>
+      <c r="C93" s="27"/>
+      <c r="D93" s="27"/>
     </row>
     <row r="94" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C94" s="23"/>
-      <c r="D94" s="23"/>
+      <c r="C94" s="27"/>
+      <c r="D94" s="27"/>
     </row>
     <row r="95" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C95" s="23"/>
-      <c r="D95" s="23"/>
+      <c r="C95" s="27"/>
+      <c r="D95" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="84">

</xml_diff>

<commit_message>
Begin adding gifts and implement basic type toggles
</commit_message>
<xml_diff>
--- a/rcc-ministry-catalog/src/main/resources/RCC Ministry Catalog.xlsx
+++ b/rcc-ministry-catalog/src/main/resources/RCC Ministry Catalog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16740" yWindow="0" windowWidth="7860" windowHeight="8565" activeTab="2"/>
+    <workbookView xWindow="18600" yWindow="0" windowWidth="7860" windowHeight="8565"/>
   </bookViews>
   <sheets>
     <sheet name="Outline" sheetId="5" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="240">
   <si>
     <t>Ministry Role:</t>
   </si>
@@ -732,6 +732,27 @@
   </si>
   <si>
     <t>Ministry Types</t>
+  </si>
+  <si>
+    <t>Interpretation</t>
+  </si>
+  <si>
+    <t>Gift 1</t>
+  </si>
+  <si>
+    <t>Gift 2</t>
+  </si>
+  <si>
+    <t>Gift 3</t>
+  </si>
+  <si>
+    <t>New Building</t>
+  </si>
+  <si>
+    <t>1.4.2</t>
+  </si>
+  <si>
+    <t>Kevin Murray</t>
   </si>
 </sst>
 </file>
@@ -906,6 +927,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -924,21 +946,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1007,8 +1028,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TDirectory" displayName="TDirectory" ref="A1:C13" totalsRowShown="0">
-  <autoFilter ref="A1:C13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TDirectory" displayName="TDirectory" ref="A1:C14" totalsRowShown="0">
+  <autoFilter ref="A1:C14"/>
   <sortState ref="A2:C13">
     <sortCondition ref="A1:A13"/>
   </sortState>
@@ -1032,6 +1053,16 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TGifts" displayName="TGifts" ref="C1:C31" totalsRowShown="0">
+  <autoFilter ref="C1:C31"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Gifts"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Lookups" displayName="Lookups" ref="F1:H31" totalsRowShown="0">
   <autoFilter ref="F1:H31"/>
   <sortState ref="F2:G31">
@@ -1309,12 +1340,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I79"/>
+  <dimension ref="A1:L80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomLeft" activeCell="J74" sqref="J74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1325,9 +1356,10 @@
     <col min="6" max="6" width="20.7109375" customWidth="1"/>
     <col min="7" max="7" width="20.7109375" style="16" customWidth="1"/>
     <col min="8" max="9" width="20.7109375" customWidth="1"/>
+    <col min="10" max="12" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>73</v>
       </c>
@@ -1355,8 +1387,17 @@
       <c r="I1" s="19" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="17">
         <v>1</v>
       </c>
@@ -1373,7 +1414,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" s="17">
         <v>1.1000000000000001</v>
       </c>
@@ -1384,23 +1425,38 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C4" s="17" t="s">
         <v>76</v>
       </c>
       <c r="D4" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C5" s="17" t="s">
         <v>79</v>
       </c>
       <c r="D5" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" s="17">
         <v>1.2</v>
       </c>
@@ -1411,31 +1467,43 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C7" s="17" t="s">
         <v>88</v>
       </c>
       <c r="D7" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C8" s="17" t="s">
         <v>89</v>
       </c>
       <c r="D8" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C9" s="17" t="s">
         <v>90</v>
       </c>
       <c r="D9" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>29</v>
+      </c>
+      <c r="K9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" s="17">
         <v>1.3</v>
       </c>
@@ -1446,649 +1514,792 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C11" s="17" t="s">
         <v>94</v>
       </c>
       <c r="D11" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>15</v>
+      </c>
+      <c r="K11" t="s">
+        <v>18</v>
+      </c>
+      <c r="L11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C12" s="17" t="s">
         <v>96</v>
       </c>
       <c r="D12" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" s="17">
         <v>1.4</v>
       </c>
       <c r="D13" t="s">
-        <v>98</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C14" s="17" t="s">
         <v>100</v>
       </c>
       <c r="D14" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="17">
+      <c r="G14" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="J14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C15" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="D15" t="s">
+        <v>98</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="17">
         <v>1.5</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>102</v>
       </c>
-      <c r="G15" s="16" t="s">
+      <c r="G16" s="16" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="17">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="17">
         <v>1.6</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="17">
+      <c r="J17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="17">
         <v>1.7</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>198</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="17">
-        <v>1.8</v>
-      </c>
-      <c r="D18" t="s">
-        <v>199</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="17">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="17">
+        <v>1.8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>199</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="17">
         <v>2</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D20" t="s">
         <v>104</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="G19" s="16" t="s">
+      <c r="G20" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H20" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="17">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="17">
         <v>2.1</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="17" t="s">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C22" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D22" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="17" t="s">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C23" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C23" s="17" t="s">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C24" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C24" s="17" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C25" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="17">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="17">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D26" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C26" s="17" t="s">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C27" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C27" s="17" t="s">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C28" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D28" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C28" s="17" t="s">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C29" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D29" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C29" s="17" t="s">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C30" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D30" t="s">
         <v>194</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C30" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D30" t="s">
-        <v>197</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="17">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C31" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D31" t="s">
+        <v>197</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B32" s="17">
         <v>2.2999999999999998</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D32" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C32" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="D32" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C33" s="17" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D33" t="s">
-        <v>201</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C34" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="D34" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C35" s="17" t="s">
         <v>200</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D35" t="s">
         <v>202</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="17">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="17">
         <v>2.4</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="17">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="17">
         <v>3</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>126</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>127</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="17">
-        <v>3.1</v>
-      </c>
-      <c r="D37" t="s">
-        <v>128</v>
-      </c>
-      <c r="G37" s="16" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B38" s="17">
+        <v>3.1</v>
+      </c>
+      <c r="D38" t="s">
+        <v>128</v>
+      </c>
+      <c r="G38" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="17">
         <v>3.2</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D39" t="s">
         <v>131</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C39" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="D39" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C40" s="17" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D40" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C41" s="17" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D41" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C42" s="17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D42" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C43" s="17" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D43" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C44" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="D44" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C45" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D45" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="17">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="17">
         <v>3.3</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D46" t="s">
         <v>144</v>
       </c>
-      <c r="G45" s="16" t="s">
+      <c r="G46" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="H45" t="s">
+      <c r="H46" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C46" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="D46" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C47" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D47" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C48" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D48" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B48" s="17">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B49" s="17">
         <v>3.4</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D49" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C49" s="17" t="s">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C50" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D50" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C50" s="17" t="s">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C51" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D51" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="17">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="17">
         <v>4</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D52" t="s">
         <v>71</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E52" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F52" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B52" s="17">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B53" s="17">
         <v>4.0999999999999996</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D53" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C53" s="17" t="s">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C54" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D54" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C54" s="17" t="s">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C55" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D55" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C55" s="17" t="s">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C56" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D56" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C56" s="17" t="s">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C57" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D57" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B57" s="17">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B58" s="17">
         <v>4.2</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D58" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C58" s="17" t="s">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C59" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D59" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C59" s="17" t="s">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C60" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D60" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="17">
+      <c r="J60" t="s">
+        <v>16</v>
+      </c>
+      <c r="K60" t="s">
+        <v>37</v>
+      </c>
+      <c r="L60" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" s="17">
         <v>5</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D61" t="s">
         <v>169</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="E61" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F61" t="s">
         <v>82</v>
       </c>
-      <c r="G60" s="16" t="s">
+      <c r="G61" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="H60" t="s">
+      <c r="H61" t="s">
         <v>212</v>
       </c>
-      <c r="I60" t="s">
+      <c r="I61" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B61" s="17">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B62" s="17">
         <v>5.0999999999999996</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D62" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C62" s="17" t="s">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C63" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D63" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C63" s="17" t="s">
+      <c r="J63" t="s">
+        <v>43</v>
+      </c>
+      <c r="K63" t="s">
+        <v>21</v>
+      </c>
+      <c r="L63" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C64" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D64" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C64" s="17" t="s">
+      <c r="J64" t="s">
+        <v>43</v>
+      </c>
+      <c r="K64" t="s">
+        <v>35</v>
+      </c>
+      <c r="L64" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C65" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D65" t="s">
         <v>203</v>
       </c>
-      <c r="E64" s="1" t="s">
+      <c r="E65" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="G64" s="16" t="s">
+      <c r="G65" s="16" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B65" s="17">
+      <c r="J65" t="s">
+        <v>43</v>
+      </c>
+      <c r="K65" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B66" s="17">
         <v>5.2</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D66" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C66" s="17" t="s">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C67" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D67" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C67" s="17" t="s">
+      <c r="J67" t="s">
+        <v>44</v>
+      </c>
+      <c r="K67" t="s">
+        <v>15</v>
+      </c>
+      <c r="L67" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C68" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D68" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C68" s="17" t="s">
+      <c r="J68" t="s">
+        <v>15</v>
+      </c>
+      <c r="K68" t="s">
+        <v>42</v>
+      </c>
+      <c r="L68" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C69" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D69" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="17">
+      <c r="J69" t="s">
+        <v>15</v>
+      </c>
+      <c r="K69" t="s">
+        <v>42</v>
+      </c>
+      <c r="L69" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" s="17">
         <v>6</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D70" t="s">
         <v>188</v>
       </c>
-      <c r="E69" s="1" t="s">
+      <c r="E70" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B70" s="17">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B71" s="17">
         <v>6.1</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D71" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B71" s="17">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B72" s="17">
         <v>6.2</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D72" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C72" s="17" t="s">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C73" s="17" t="s">
         <v>182</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D73" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C73" s="17" t="s">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C74" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D74" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C74" s="17" t="s">
+      <c r="J74" t="s">
+        <v>20</v>
+      </c>
+      <c r="K74" t="s">
+        <v>31</v>
+      </c>
+      <c r="L74" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C75" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D75" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="17">
+      <c r="J75" t="s">
+        <v>15</v>
+      </c>
+      <c r="K75" t="s">
+        <v>34</v>
+      </c>
+      <c r="L75" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A76" s="17">
         <v>7</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D76" t="s">
         <v>32</v>
       </c>
-      <c r="E75" s="1" t="s">
+      <c r="E76" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="G75" s="16" t="s">
+      <c r="G76" s="16" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B76" s="17">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B77" s="17">
         <v>7.1</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D77" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B77" s="17">
+      <c r="J77" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B78" s="17">
         <v>7.2</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D78" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B78" s="17">
+      <c r="J78" t="s">
+        <v>32</v>
+      </c>
+      <c r="K78" t="s">
+        <v>41</v>
+      </c>
+      <c r="L78" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B79" s="17">
         <v>7.3</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D79" t="s">
         <v>206</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B79" s="17">
-        <v>7.4</v>
-      </c>
-      <c r="D79" t="s">
-        <v>207</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>195</v>
       </c>
+      <c r="J79" t="s">
+        <v>32</v>
+      </c>
+      <c r="K79" t="s">
+        <v>35</v>
+      </c>
+      <c r="L79" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B80" s="17">
+        <v>7.4</v>
+      </c>
+      <c r="D80" t="s">
+        <v>207</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="J80" t="s">
+        <v>32</v>
+      </c>
+      <c r="K80" t="s">
+        <v>15</v>
+      </c>
+      <c r="L80" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Not in directory" error="You have entered a person who is not in the Directory tab" sqref="G2:I200">
+  <dataValidations count="3">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Not in directory" error="You have entered a person who is not in the Directory tab" sqref="G2:I201">
       <formula1>INDIRECT("TDirectory[Name]")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E220">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E221">
       <formula1>INDIRECT("TMinistryTypes[Ministry Types]")</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:L201">
+      <formula1>INDIRECT("TGifts[Gifts]")</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2098,10 +2309,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2202,25 +2413,33 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B11" t="s">
-        <v>221</v>
+        <v>239</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>130</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>228</v>
+        <v>82</v>
+      </c>
+      <c r="B12" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>154</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B14" s="20" t="s">
         <v>225</v>
       </c>
     </row>
@@ -2239,36 +2458,187 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>195</v>
       </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2295,10 +2665,10 @@
         <f>Reference!A1</f>
         <v>Ministry Role:</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="23"/>
+      <c r="D1" s="24"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2315,10 +2685,10 @@
         <f>Reference!A3</f>
         <v>Filled by:</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="25"/>
+      <c r="D3" s="26"/>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2329,11 +2699,11 @@
         <f>Reference!A5</f>
         <v>In Ministry Area:</v>
       </c>
-      <c r="C5" s="26" t="e">
+      <c r="C5" s="27" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="D5" s="26"/>
+      <c r="D5" s="27"/>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2341,11 +2711,11 @@
         <f>Reference!A6</f>
         <v>Under Ministry Role:</v>
       </c>
-      <c r="C6" s="26" t="e">
+      <c r="C6" s="27" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="D6" s="26"/>
+      <c r="D6" s="27"/>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2376,10 +2746,10 @@
         <f>Reference!A10</f>
         <v>Position open to:</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="D10" s="25"/>
+      <c r="D10" s="26"/>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" ht="8.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2388,31 +2758,31 @@
         <f>Reference!A12</f>
         <v>Relevant gifts:</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="22"/>
+      <c r="D12" s="23"/>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="22"/>
+      <c r="D13" s="23"/>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="22"/>
+      <c r="D14" s="23"/>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="22"/>
+      <c r="D15" s="23"/>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2426,32 +2796,32 @@
         <f>Reference!A19</f>
         <v>Relevant skills:</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="22"/>
+      <c r="D17" s="23"/>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="22"/>
+      <c r="D18" s="23"/>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="D19" s="22"/>
+      <c r="D19" s="23"/>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="D20" s="22"/>
+      <c r="D20" s="23"/>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2465,24 +2835,24 @@
         <f>Reference!A25</f>
         <v>Personality:</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="D22" s="22"/>
+      <c r="D22" s="23"/>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="21" t="s">
+      <c r="C23" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="22"/>
+      <c r="D23" s="23"/>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="21" t="s">
+      <c r="C24" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="D24" s="22"/>
+      <c r="D24" s="23"/>
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2495,10 +2865,10 @@
         <f>Reference!A31</f>
         <v>Length of service:</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C26" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="D26" s="22"/>
+      <c r="D26" s="23"/>
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -2506,17 +2876,17 @@
         <f>Reference!A32</f>
         <v>Time commitments:</v>
       </c>
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="D27" s="22"/>
+      <c r="D27" s="23"/>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C28" s="21" t="s">
+      <c r="C28" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="22"/>
+      <c r="D28" s="23"/>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2529,246 +2899,309 @@
         <f>Reference!A38</f>
         <v>Responsibilities:</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C30" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="D30" s="22"/>
+      <c r="D30" s="23"/>
       <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C31" s="21" t="s">
+      <c r="C31" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="D31" s="22"/>
+      <c r="D31" s="23"/>
       <c r="E31" s="5"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C32" s="21" t="s">
+      <c r="C32" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="D32" s="22"/>
+      <c r="D32" s="23"/>
       <c r="E32" s="5"/>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C33" s="21" t="s">
+      <c r="C33" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="D33" s="22"/>
+      <c r="D33" s="23"/>
       <c r="E33" s="5"/>
     </row>
     <row r="34" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C34" s="21" t="s">
+      <c r="C34" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="D34" s="22"/>
+      <c r="D34" s="23"/>
       <c r="E34" s="5"/>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
     </row>
     <row r="36" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C36" s="27"/>
-      <c r="D36" s="27"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C37" s="27"/>
-      <c r="D37" s="27"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C38" s="27"/>
-      <c r="D38" s="27"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C39" s="27"/>
-      <c r="D39" s="27"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
     </row>
     <row r="40" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C40" s="27"/>
-      <c r="D40" s="27"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C41" s="27"/>
-      <c r="D41" s="27"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
     </row>
     <row r="42" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C42" s="27"/>
-      <c r="D42" s="27"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
     </row>
     <row r="43" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C43" s="27"/>
-      <c r="D43" s="27"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="21"/>
     </row>
     <row r="44" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C44" s="27"/>
-      <c r="D44" s="27"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="21"/>
     </row>
     <row r="45" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C45" s="27"/>
-      <c r="D45" s="27"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
     </row>
     <row r="46" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C46" s="27"/>
-      <c r="D46" s="27"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
     </row>
     <row r="47" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="21"/>
     </row>
     <row r="48" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C48" s="27"/>
-      <c r="D48" s="27"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="21"/>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C49" s="27"/>
-      <c r="D49" s="27"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C50" s="27"/>
-      <c r="D50" s="27"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="21"/>
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C51" s="27"/>
-      <c r="D51" s="27"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="21"/>
     </row>
     <row r="52" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C52" s="27"/>
-      <c r="D52" s="27"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="21"/>
     </row>
     <row r="53" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C53" s="27"/>
-      <c r="D53" s="27"/>
+      <c r="C53" s="21"/>
+      <c r="D53" s="21"/>
     </row>
     <row r="54" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C54" s="27"/>
-      <c r="D54" s="27"/>
+      <c r="C54" s="21"/>
+      <c r="D54" s="21"/>
     </row>
     <row r="55" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C55" s="27"/>
-      <c r="D55" s="27"/>
+      <c r="C55" s="21"/>
+      <c r="D55" s="21"/>
     </row>
     <row r="56" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C56" s="27"/>
-      <c r="D56" s="27"/>
+      <c r="C56" s="21"/>
+      <c r="D56" s="21"/>
     </row>
     <row r="57" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C57" s="27"/>
-      <c r="D57" s="27"/>
+      <c r="C57" s="21"/>
+      <c r="D57" s="21"/>
     </row>
     <row r="58" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C58" s="27"/>
-      <c r="D58" s="27"/>
+      <c r="C58" s="21"/>
+      <c r="D58" s="21"/>
     </row>
     <row r="59" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C59" s="27"/>
-      <c r="D59" s="27"/>
+      <c r="C59" s="21"/>
+      <c r="D59" s="21"/>
     </row>
     <row r="60" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C60" s="27"/>
-      <c r="D60" s="27"/>
+      <c r="C60" s="21"/>
+      <c r="D60" s="21"/>
     </row>
     <row r="61" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C61" s="27"/>
-      <c r="D61" s="27"/>
+      <c r="C61" s="21"/>
+      <c r="D61" s="21"/>
     </row>
     <row r="62" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C62" s="27"/>
-      <c r="D62" s="27"/>
+      <c r="C62" s="21"/>
+      <c r="D62" s="21"/>
     </row>
     <row r="63" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C63" s="27"/>
-      <c r="D63" s="27"/>
+      <c r="C63" s="21"/>
+      <c r="D63" s="21"/>
     </row>
     <row r="64" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C64" s="27"/>
-      <c r="D64" s="27"/>
+      <c r="C64" s="21"/>
+      <c r="D64" s="21"/>
     </row>
     <row r="65" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C65" s="27"/>
-      <c r="D65" s="27"/>
+      <c r="C65" s="21"/>
+      <c r="D65" s="21"/>
     </row>
     <row r="66" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C66" s="27"/>
-      <c r="D66" s="27"/>
+      <c r="C66" s="21"/>
+      <c r="D66" s="21"/>
     </row>
     <row r="67" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C67" s="27"/>
-      <c r="D67" s="27"/>
+      <c r="C67" s="21"/>
+      <c r="D67" s="21"/>
     </row>
     <row r="68" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C68" s="27"/>
-      <c r="D68" s="27"/>
+      <c r="C68" s="21"/>
+      <c r="D68" s="21"/>
     </row>
     <row r="69" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C69" s="27"/>
-      <c r="D69" s="27"/>
+      <c r="C69" s="21"/>
+      <c r="D69" s="21"/>
     </row>
     <row r="70" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C70" s="27"/>
-      <c r="D70" s="27"/>
+      <c r="C70" s="21"/>
+      <c r="D70" s="21"/>
     </row>
     <row r="71" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C71" s="27"/>
-      <c r="D71" s="27"/>
+      <c r="C71" s="21"/>
+      <c r="D71" s="21"/>
     </row>
     <row r="72" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C72" s="27"/>
-      <c r="D72" s="27"/>
+      <c r="C72" s="21"/>
+      <c r="D72" s="21"/>
     </row>
     <row r="73" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C73" s="27"/>
-      <c r="D73" s="27"/>
+      <c r="C73" s="21"/>
+      <c r="D73" s="21"/>
     </row>
     <row r="74" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C74" s="27"/>
-      <c r="D74" s="27"/>
+      <c r="C74" s="21"/>
+      <c r="D74" s="21"/>
     </row>
     <row r="75" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C75" s="27"/>
-      <c r="D75" s="27"/>
+      <c r="C75" s="21"/>
+      <c r="D75" s="21"/>
     </row>
     <row r="76" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C76" s="27"/>
-      <c r="D76" s="27"/>
+      <c r="C76" s="21"/>
+      <c r="D76" s="21"/>
     </row>
     <row r="77" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C77" s="27"/>
-      <c r="D77" s="27"/>
+      <c r="C77" s="21"/>
+      <c r="D77" s="21"/>
     </row>
     <row r="78" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C78" s="27"/>
-      <c r="D78" s="27"/>
+      <c r="C78" s="21"/>
+      <c r="D78" s="21"/>
     </row>
     <row r="79" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C79" s="27"/>
-      <c r="D79" s="27"/>
+      <c r="C79" s="21"/>
+      <c r="D79" s="21"/>
     </row>
     <row r="80" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C80" s="27"/>
-      <c r="D80" s="27"/>
+      <c r="C80" s="21"/>
+      <c r="D80" s="21"/>
     </row>
     <row r="81" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C81" s="27"/>
-      <c r="D81" s="27"/>
+      <c r="C81" s="21"/>
+      <c r="D81" s="21"/>
     </row>
     <row r="82" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C82" s="27"/>
-      <c r="D82" s="27"/>
+      <c r="C82" s="21"/>
+      <c r="D82" s="21"/>
     </row>
     <row r="83" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C83" s="27"/>
-      <c r="D83" s="27"/>
+      <c r="C83" s="21"/>
+      <c r="D83" s="21"/>
     </row>
     <row r="84" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C84" s="27"/>
-      <c r="D84" s="27"/>
+      <c r="C84" s="21"/>
+      <c r="D84" s="21"/>
     </row>
     <row r="85" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C85" s="27"/>
-      <c r="D85" s="27"/>
+      <c r="C85" s="21"/>
+      <c r="D85" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="75">
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="C72:D72"/>
     <mergeCell ref="C85:D85"/>
     <mergeCell ref="C74:D74"/>
     <mergeCell ref="C75:D75"/>
@@ -2781,69 +3214,6 @@
     <mergeCell ref="C82:D82"/>
     <mergeCell ref="C83:D83"/>
     <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C10:D10"/>
   </mergeCells>
   <conditionalFormatting sqref="C2">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
@@ -2903,8 +3273,8 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
       <c r="E1" s="1"/>
       <c r="F1" t="s">
         <v>45</v>
@@ -2963,8 +3333,8 @@
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
       <c r="E5" s="2"/>
       <c r="G5" t="s">
         <v>29</v>
@@ -2974,8 +3344,8 @@
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
       <c r="E6" s="2"/>
       <c r="G6" t="s">
         <v>23</v>
@@ -3262,241 +3632,309 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
-      <c r="C39" s="32"/>
-      <c r="D39" s="33"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="31"/>
       <c r="E39" s="5"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C40" s="32"/>
-      <c r="D40" s="33"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="31"/>
       <c r="E40" s="5"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C41" s="32"/>
-      <c r="D41" s="33"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="31"/>
       <c r="E41" s="5"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C42" s="32"/>
-      <c r="D42" s="33"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="31"/>
       <c r="E42" s="5"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C43" s="32"/>
-      <c r="D43" s="33"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="31"/>
       <c r="E43" s="5"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C44" s="32"/>
-      <c r="D44" s="33"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="31"/>
       <c r="E44" s="5"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C45" s="27"/>
-      <c r="D45" s="27"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C46" s="27"/>
-      <c r="D46" s="27"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="21"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C48" s="27"/>
-      <c r="D48" s="27"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="21"/>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C49" s="27"/>
-      <c r="D49" s="27"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C50" s="27"/>
-      <c r="D50" s="27"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="21"/>
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C51" s="27"/>
-      <c r="D51" s="27"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="21"/>
     </row>
     <row r="52" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C52" s="27"/>
-      <c r="D52" s="27"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="21"/>
     </row>
     <row r="53" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C53" s="27"/>
-      <c r="D53" s="27"/>
+      <c r="C53" s="21"/>
+      <c r="D53" s="21"/>
     </row>
     <row r="54" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C54" s="27"/>
-      <c r="D54" s="27"/>
+      <c r="C54" s="21"/>
+      <c r="D54" s="21"/>
     </row>
     <row r="55" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C55" s="27"/>
-      <c r="D55" s="27"/>
+      <c r="C55" s="21"/>
+      <c r="D55" s="21"/>
     </row>
     <row r="56" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C56" s="27"/>
-      <c r="D56" s="27"/>
+      <c r="C56" s="21"/>
+      <c r="D56" s="21"/>
     </row>
     <row r="57" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C57" s="27"/>
-      <c r="D57" s="27"/>
+      <c r="C57" s="21"/>
+      <c r="D57" s="21"/>
     </row>
     <row r="58" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C58" s="27"/>
-      <c r="D58" s="27"/>
+      <c r="C58" s="21"/>
+      <c r="D58" s="21"/>
     </row>
     <row r="59" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C59" s="27"/>
-      <c r="D59" s="27"/>
+      <c r="C59" s="21"/>
+      <c r="D59" s="21"/>
     </row>
     <row r="60" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C60" s="27"/>
-      <c r="D60" s="27"/>
+      <c r="C60" s="21"/>
+      <c r="D60" s="21"/>
     </row>
     <row r="61" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C61" s="27"/>
-      <c r="D61" s="27"/>
+      <c r="C61" s="21"/>
+      <c r="D61" s="21"/>
     </row>
     <row r="62" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C62" s="27"/>
-      <c r="D62" s="27"/>
+      <c r="C62" s="21"/>
+      <c r="D62" s="21"/>
     </row>
     <row r="63" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C63" s="27"/>
-      <c r="D63" s="27"/>
+      <c r="C63" s="21"/>
+      <c r="D63" s="21"/>
     </row>
     <row r="64" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C64" s="27"/>
-      <c r="D64" s="27"/>
+      <c r="C64" s="21"/>
+      <c r="D64" s="21"/>
     </row>
     <row r="65" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C65" s="27"/>
-      <c r="D65" s="27"/>
+      <c r="C65" s="21"/>
+      <c r="D65" s="21"/>
     </row>
     <row r="66" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C66" s="27"/>
-      <c r="D66" s="27"/>
+      <c r="C66" s="21"/>
+      <c r="D66" s="21"/>
     </row>
     <row r="67" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C67" s="27"/>
-      <c r="D67" s="27"/>
+      <c r="C67" s="21"/>
+      <c r="D67" s="21"/>
     </row>
     <row r="68" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C68" s="27"/>
-      <c r="D68" s="27"/>
+      <c r="C68" s="21"/>
+      <c r="D68" s="21"/>
     </row>
     <row r="69" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C69" s="27"/>
-      <c r="D69" s="27"/>
+      <c r="C69" s="21"/>
+      <c r="D69" s="21"/>
     </row>
     <row r="70" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C70" s="27"/>
-      <c r="D70" s="27"/>
+      <c r="C70" s="21"/>
+      <c r="D70" s="21"/>
     </row>
     <row r="71" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C71" s="27"/>
-      <c r="D71" s="27"/>
+      <c r="C71" s="21"/>
+      <c r="D71" s="21"/>
     </row>
     <row r="72" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C72" s="27"/>
-      <c r="D72" s="27"/>
+      <c r="C72" s="21"/>
+      <c r="D72" s="21"/>
     </row>
     <row r="73" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C73" s="27"/>
-      <c r="D73" s="27"/>
+      <c r="C73" s="21"/>
+      <c r="D73" s="21"/>
     </row>
     <row r="74" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C74" s="27"/>
-      <c r="D74" s="27"/>
+      <c r="C74" s="21"/>
+      <c r="D74" s="21"/>
     </row>
     <row r="75" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C75" s="27"/>
-      <c r="D75" s="27"/>
+      <c r="C75" s="21"/>
+      <c r="D75" s="21"/>
     </row>
     <row r="76" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C76" s="27"/>
-      <c r="D76" s="27"/>
+      <c r="C76" s="21"/>
+      <c r="D76" s="21"/>
     </row>
     <row r="77" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C77" s="27"/>
-      <c r="D77" s="27"/>
+      <c r="C77" s="21"/>
+      <c r="D77" s="21"/>
     </row>
     <row r="78" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C78" s="27"/>
-      <c r="D78" s="27"/>
+      <c r="C78" s="21"/>
+      <c r="D78" s="21"/>
     </row>
     <row r="79" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C79" s="27"/>
-      <c r="D79" s="27"/>
+      <c r="C79" s="21"/>
+      <c r="D79" s="21"/>
     </row>
     <row r="80" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C80" s="27"/>
-      <c r="D80" s="27"/>
+      <c r="C80" s="21"/>
+      <c r="D80" s="21"/>
     </row>
     <row r="81" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C81" s="27"/>
-      <c r="D81" s="27"/>
+      <c r="C81" s="21"/>
+      <c r="D81" s="21"/>
     </row>
     <row r="82" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C82" s="27"/>
-      <c r="D82" s="27"/>
+      <c r="C82" s="21"/>
+      <c r="D82" s="21"/>
     </row>
     <row r="83" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C83" s="27"/>
-      <c r="D83" s="27"/>
+      <c r="C83" s="21"/>
+      <c r="D83" s="21"/>
     </row>
     <row r="84" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C84" s="27"/>
-      <c r="D84" s="27"/>
+      <c r="C84" s="21"/>
+      <c r="D84" s="21"/>
     </row>
     <row r="85" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C85" s="27"/>
-      <c r="D85" s="27"/>
+      <c r="C85" s="21"/>
+      <c r="D85" s="21"/>
     </row>
     <row r="86" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C86" s="27"/>
-      <c r="D86" s="27"/>
+      <c r="C86" s="21"/>
+      <c r="D86" s="21"/>
     </row>
     <row r="87" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C87" s="27"/>
-      <c r="D87" s="27"/>
+      <c r="C87" s="21"/>
+      <c r="D87" s="21"/>
     </row>
     <row r="88" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C88" s="27"/>
-      <c r="D88" s="27"/>
+      <c r="C88" s="21"/>
+      <c r="D88" s="21"/>
     </row>
     <row r="89" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C89" s="27"/>
-      <c r="D89" s="27"/>
+      <c r="C89" s="21"/>
+      <c r="D89" s="21"/>
     </row>
     <row r="90" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C90" s="27"/>
-      <c r="D90" s="27"/>
+      <c r="C90" s="21"/>
+      <c r="D90" s="21"/>
     </row>
     <row r="91" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C91" s="27"/>
-      <c r="D91" s="27"/>
+      <c r="C91" s="21"/>
+      <c r="D91" s="21"/>
     </row>
     <row r="92" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C92" s="27"/>
-      <c r="D92" s="27"/>
+      <c r="C92" s="21"/>
+      <c r="D92" s="21"/>
     </row>
     <row r="93" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C93" s="27"/>
-      <c r="D93" s="27"/>
+      <c r="C93" s="21"/>
+      <c r="D93" s="21"/>
     </row>
     <row r="94" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C94" s="27"/>
-      <c r="D94" s="27"/>
+      <c r="C94" s="21"/>
+      <c r="D94" s="21"/>
     </row>
     <row r="95" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C95" s="27"/>
-      <c r="D95" s="27"/>
+      <c r="C95" s="21"/>
+      <c r="D95" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="84">
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C81:D81"/>
     <mergeCell ref="C94:D94"/>
     <mergeCell ref="C95:D95"/>
     <mergeCell ref="C10:D10"/>
@@ -3513,74 +3951,6 @@
     <mergeCell ref="C86:D86"/>
     <mergeCell ref="C87:D87"/>
     <mergeCell ref="C76:D76"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
   </mergeCells>
   <conditionalFormatting sqref="C2">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">

</xml_diff>

<commit_message>
Only apply CSS class to leafs, reduce size of POC, begin integrating gifts
</commit_message>
<xml_diff>
--- a/rcc-ministry-catalog/src/main/resources/RCC Ministry Catalog.xlsx
+++ b/rcc-ministry-catalog/src/main/resources/RCC Ministry Catalog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="18600" yWindow="0" windowWidth="7860" windowHeight="8565"/>
+    <workbookView xWindow="20460" yWindow="0" windowWidth="7860" windowHeight="8565"/>
   </bookViews>
   <sheets>
     <sheet name="Outline" sheetId="5" r:id="rId1"/>
@@ -927,7 +927,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -946,20 +945,21 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1343,9 +1343,9 @@
   <dimension ref="A1:L80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
-      <selection pane="bottomLeft" activeCell="J74" sqref="J74"/>
+      <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2312,7 +2312,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2665,10 +2665,10 @@
         <f>Reference!A1</f>
         <v>Ministry Role:</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="24"/>
+      <c r="D1" s="23"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2685,10 +2685,10 @@
         <f>Reference!A3</f>
         <v>Filled by:</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="26"/>
+      <c r="D3" s="25"/>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2699,11 +2699,11 @@
         <f>Reference!A5</f>
         <v>In Ministry Area:</v>
       </c>
-      <c r="C5" s="27" t="e">
+      <c r="C5" s="26" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="D5" s="27"/>
+      <c r="D5" s="26"/>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2711,11 +2711,11 @@
         <f>Reference!A6</f>
         <v>Under Ministry Role:</v>
       </c>
-      <c r="C6" s="27" t="e">
+      <c r="C6" s="26" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="D6" s="27"/>
+      <c r="D6" s="26"/>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2746,10 +2746,10 @@
         <f>Reference!A10</f>
         <v>Position open to:</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="D10" s="26"/>
+      <c r="D10" s="25"/>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" ht="8.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2758,31 +2758,31 @@
         <f>Reference!A12</f>
         <v>Relevant gifts:</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="23"/>
+      <c r="D12" s="22"/>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="23"/>
+      <c r="D13" s="22"/>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="23"/>
+      <c r="D14" s="22"/>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="23"/>
+      <c r="D15" s="22"/>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2796,32 +2796,32 @@
         <f>Reference!A19</f>
         <v>Relevant skills:</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="23"/>
+      <c r="D17" s="22"/>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="23"/>
+      <c r="D18" s="22"/>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="D19" s="23"/>
+      <c r="D19" s="22"/>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="22" t="s">
+      <c r="C20" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D20" s="23"/>
+      <c r="D20" s="22"/>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2835,24 +2835,24 @@
         <f>Reference!A25</f>
         <v>Personality:</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="C22" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="D22" s="23"/>
+      <c r="D22" s="22"/>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="23"/>
+      <c r="D23" s="22"/>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="22" t="s">
+      <c r="C24" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="D24" s="23"/>
+      <c r="D24" s="22"/>
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2865,10 +2865,10 @@
         <f>Reference!A31</f>
         <v>Length of service:</v>
       </c>
-      <c r="C26" s="22" t="s">
+      <c r="C26" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="D26" s="23"/>
+      <c r="D26" s="22"/>
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -2876,17 +2876,17 @@
         <f>Reference!A32</f>
         <v>Time commitments:</v>
       </c>
-      <c r="C27" s="22" t="s">
+      <c r="C27" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="D27" s="23"/>
+      <c r="D27" s="22"/>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C28" s="22" t="s">
+      <c r="C28" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="23"/>
+      <c r="D28" s="22"/>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2899,273 +2899,282 @@
         <f>Reference!A38</f>
         <v>Responsibilities:</v>
       </c>
-      <c r="C30" s="22" t="s">
+      <c r="C30" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="D30" s="23"/>
+      <c r="D30" s="22"/>
       <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C31" s="22" t="s">
+      <c r="C31" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="D31" s="23"/>
+      <c r="D31" s="22"/>
       <c r="E31" s="5"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C32" s="22" t="s">
+      <c r="C32" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="D32" s="23"/>
+      <c r="D32" s="22"/>
       <c r="E32" s="5"/>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C33" s="22" t="s">
+      <c r="C33" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="D33" s="23"/>
+      <c r="D33" s="22"/>
       <c r="E33" s="5"/>
     </row>
     <row r="34" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C34" s="22" t="s">
+      <c r="C34" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="D34" s="23"/>
+      <c r="D34" s="22"/>
       <c r="E34" s="5"/>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
     </row>
     <row r="36" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
     </row>
     <row r="40" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C41" s="21"/>
-      <c r="D41" s="21"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27"/>
     </row>
     <row r="42" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="27"/>
     </row>
     <row r="43" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C43" s="21"/>
-      <c r="D43" s="21"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
     </row>
     <row r="44" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27"/>
     </row>
     <row r="45" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C45" s="21"/>
-      <c r="D45" s="21"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="27"/>
     </row>
     <row r="46" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="27"/>
     </row>
     <row r="47" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
     </row>
     <row r="48" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C48" s="21"/>
-      <c r="D48" s="21"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="27"/>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C49" s="21"/>
-      <c r="D49" s="21"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="27"/>
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="27"/>
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C51" s="21"/>
-      <c r="D51" s="21"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="27"/>
     </row>
     <row r="52" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
+      <c r="C52" s="27"/>
+      <c r="D52" s="27"/>
     </row>
     <row r="53" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C53" s="21"/>
-      <c r="D53" s="21"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="27"/>
     </row>
     <row r="54" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C54" s="21"/>
-      <c r="D54" s="21"/>
+      <c r="C54" s="27"/>
+      <c r="D54" s="27"/>
     </row>
     <row r="55" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C55" s="21"/>
-      <c r="D55" s="21"/>
+      <c r="C55" s="27"/>
+      <c r="D55" s="27"/>
     </row>
     <row r="56" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C56" s="21"/>
-      <c r="D56" s="21"/>
+      <c r="C56" s="27"/>
+      <c r="D56" s="27"/>
     </row>
     <row r="57" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C57" s="21"/>
-      <c r="D57" s="21"/>
+      <c r="C57" s="27"/>
+      <c r="D57" s="27"/>
     </row>
     <row r="58" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C58" s="21"/>
-      <c r="D58" s="21"/>
+      <c r="C58" s="27"/>
+      <c r="D58" s="27"/>
     </row>
     <row r="59" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C59" s="21"/>
-      <c r="D59" s="21"/>
+      <c r="C59" s="27"/>
+      <c r="D59" s="27"/>
     </row>
     <row r="60" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C60" s="21"/>
-      <c r="D60" s="21"/>
+      <c r="C60" s="27"/>
+      <c r="D60" s="27"/>
     </row>
     <row r="61" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C61" s="21"/>
-      <c r="D61" s="21"/>
+      <c r="C61" s="27"/>
+      <c r="D61" s="27"/>
     </row>
     <row r="62" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C62" s="21"/>
-      <c r="D62" s="21"/>
+      <c r="C62" s="27"/>
+      <c r="D62" s="27"/>
     </row>
     <row r="63" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C63" s="21"/>
-      <c r="D63" s="21"/>
+      <c r="C63" s="27"/>
+      <c r="D63" s="27"/>
     </row>
     <row r="64" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C64" s="21"/>
-      <c r="D64" s="21"/>
+      <c r="C64" s="27"/>
+      <c r="D64" s="27"/>
     </row>
     <row r="65" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C65" s="21"/>
-      <c r="D65" s="21"/>
+      <c r="C65" s="27"/>
+      <c r="D65" s="27"/>
     </row>
     <row r="66" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C66" s="21"/>
-      <c r="D66" s="21"/>
+      <c r="C66" s="27"/>
+      <c r="D66" s="27"/>
     </row>
     <row r="67" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C67" s="21"/>
-      <c r="D67" s="21"/>
+      <c r="C67" s="27"/>
+      <c r="D67" s="27"/>
     </row>
     <row r="68" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C68" s="21"/>
-      <c r="D68" s="21"/>
+      <c r="C68" s="27"/>
+      <c r="D68" s="27"/>
     </row>
     <row r="69" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C69" s="21"/>
-      <c r="D69" s="21"/>
+      <c r="C69" s="27"/>
+      <c r="D69" s="27"/>
     </row>
     <row r="70" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C70" s="21"/>
-      <c r="D70" s="21"/>
+      <c r="C70" s="27"/>
+      <c r="D70" s="27"/>
     </row>
     <row r="71" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C71" s="21"/>
-      <c r="D71" s="21"/>
+      <c r="C71" s="27"/>
+      <c r="D71" s="27"/>
     </row>
     <row r="72" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C72" s="21"/>
-      <c r="D72" s="21"/>
+      <c r="C72" s="27"/>
+      <c r="D72" s="27"/>
     </row>
     <row r="73" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C73" s="21"/>
-      <c r="D73" s="21"/>
+      <c r="C73" s="27"/>
+      <c r="D73" s="27"/>
     </row>
     <row r="74" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C74" s="21"/>
-      <c r="D74" s="21"/>
+      <c r="C74" s="27"/>
+      <c r="D74" s="27"/>
     </row>
     <row r="75" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C75" s="21"/>
-      <c r="D75" s="21"/>
+      <c r="C75" s="27"/>
+      <c r="D75" s="27"/>
     </row>
     <row r="76" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C76" s="21"/>
-      <c r="D76" s="21"/>
+      <c r="C76" s="27"/>
+      <c r="D76" s="27"/>
     </row>
     <row r="77" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C77" s="21"/>
-      <c r="D77" s="21"/>
+      <c r="C77" s="27"/>
+      <c r="D77" s="27"/>
     </row>
     <row r="78" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C78" s="21"/>
-      <c r="D78" s="21"/>
+      <c r="C78" s="27"/>
+      <c r="D78" s="27"/>
     </row>
     <row r="79" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C79" s="21"/>
-      <c r="D79" s="21"/>
+      <c r="C79" s="27"/>
+      <c r="D79" s="27"/>
     </row>
     <row r="80" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C80" s="21"/>
-      <c r="D80" s="21"/>
+      <c r="C80" s="27"/>
+      <c r="D80" s="27"/>
     </row>
     <row r="81" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C81" s="21"/>
-      <c r="D81" s="21"/>
+      <c r="C81" s="27"/>
+      <c r="D81" s="27"/>
     </row>
     <row r="82" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C82" s="21"/>
-      <c r="D82" s="21"/>
+      <c r="C82" s="27"/>
+      <c r="D82" s="27"/>
     </row>
     <row r="83" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C83" s="21"/>
-      <c r="D83" s="21"/>
+      <c r="C83" s="27"/>
+      <c r="D83" s="27"/>
     </row>
     <row r="84" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C84" s="21"/>
-      <c r="D84" s="21"/>
+      <c r="C84" s="27"/>
+      <c r="D84" s="27"/>
     </row>
     <row r="85" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C85" s="21"/>
-      <c r="D85" s="21"/>
+      <c r="C85" s="27"/>
+      <c r="D85" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C60:D60"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="C38:D38"/>
     <mergeCell ref="C39:D39"/>
@@ -3178,42 +3187,33 @@
     <mergeCell ref="C46:D46"/>
     <mergeCell ref="C47:D47"/>
     <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C10:D10"/>
   </mergeCells>
   <conditionalFormatting sqref="C2">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
@@ -3273,8 +3273,8 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
       <c r="E1" s="1"/>
       <c r="F1" t="s">
         <v>45</v>
@@ -3333,8 +3333,8 @@
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
       <c r="E5" s="2"/>
       <c r="G5" t="s">
         <v>29</v>
@@ -3344,8 +3344,8 @@
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
       <c r="E6" s="2"/>
       <c r="G6" t="s">
         <v>23</v>
@@ -3632,309 +3632,241 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="31"/>
+      <c r="C39" s="32"/>
+      <c r="D39" s="33"/>
       <c r="E39" s="5"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C40" s="30"/>
-      <c r="D40" s="31"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="33"/>
       <c r="E40" s="5"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C41" s="30"/>
-      <c r="D41" s="31"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="33"/>
       <c r="E41" s="5"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C42" s="30"/>
-      <c r="D42" s="31"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="33"/>
       <c r="E42" s="5"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C43" s="30"/>
-      <c r="D43" s="31"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="33"/>
       <c r="E43" s="5"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C44" s="30"/>
-      <c r="D44" s="31"/>
+      <c r="C44" s="32"/>
+      <c r="D44" s="33"/>
       <c r="E44" s="5"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C45" s="21"/>
-      <c r="D45" s="21"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="27"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="27"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C48" s="21"/>
-      <c r="D48" s="21"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="27"/>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C49" s="21"/>
-      <c r="D49" s="21"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="27"/>
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="27"/>
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C51" s="21"/>
-      <c r="D51" s="21"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="27"/>
     </row>
     <row r="52" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
+      <c r="C52" s="27"/>
+      <c r="D52" s="27"/>
     </row>
     <row r="53" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C53" s="21"/>
-      <c r="D53" s="21"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="27"/>
     </row>
     <row r="54" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C54" s="21"/>
-      <c r="D54" s="21"/>
+      <c r="C54" s="27"/>
+      <c r="D54" s="27"/>
     </row>
     <row r="55" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C55" s="21"/>
-      <c r="D55" s="21"/>
+      <c r="C55" s="27"/>
+      <c r="D55" s="27"/>
     </row>
     <row r="56" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C56" s="21"/>
-      <c r="D56" s="21"/>
+      <c r="C56" s="27"/>
+      <c r="D56" s="27"/>
     </row>
     <row r="57" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C57" s="21"/>
-      <c r="D57" s="21"/>
+      <c r="C57" s="27"/>
+      <c r="D57" s="27"/>
     </row>
     <row r="58" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C58" s="21"/>
-      <c r="D58" s="21"/>
+      <c r="C58" s="27"/>
+      <c r="D58" s="27"/>
     </row>
     <row r="59" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C59" s="21"/>
-      <c r="D59" s="21"/>
+      <c r="C59" s="27"/>
+      <c r="D59" s="27"/>
     </row>
     <row r="60" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C60" s="21"/>
-      <c r="D60" s="21"/>
+      <c r="C60" s="27"/>
+      <c r="D60" s="27"/>
     </row>
     <row r="61" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C61" s="21"/>
-      <c r="D61" s="21"/>
+      <c r="C61" s="27"/>
+      <c r="D61" s="27"/>
     </row>
     <row r="62" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C62" s="21"/>
-      <c r="D62" s="21"/>
+      <c r="C62" s="27"/>
+      <c r="D62" s="27"/>
     </row>
     <row r="63" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C63" s="21"/>
-      <c r="D63" s="21"/>
+      <c r="C63" s="27"/>
+      <c r="D63" s="27"/>
     </row>
     <row r="64" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C64" s="21"/>
-      <c r="D64" s="21"/>
+      <c r="C64" s="27"/>
+      <c r="D64" s="27"/>
     </row>
     <row r="65" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C65" s="21"/>
-      <c r="D65" s="21"/>
+      <c r="C65" s="27"/>
+      <c r="D65" s="27"/>
     </row>
     <row r="66" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C66" s="21"/>
-      <c r="D66" s="21"/>
+      <c r="C66" s="27"/>
+      <c r="D66" s="27"/>
     </row>
     <row r="67" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C67" s="21"/>
-      <c r="D67" s="21"/>
+      <c r="C67" s="27"/>
+      <c r="D67" s="27"/>
     </row>
     <row r="68" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C68" s="21"/>
-      <c r="D68" s="21"/>
+      <c r="C68" s="27"/>
+      <c r="D68" s="27"/>
     </row>
     <row r="69" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C69" s="21"/>
-      <c r="D69" s="21"/>
+      <c r="C69" s="27"/>
+      <c r="D69" s="27"/>
     </row>
     <row r="70" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C70" s="21"/>
-      <c r="D70" s="21"/>
+      <c r="C70" s="27"/>
+      <c r="D70" s="27"/>
     </row>
     <row r="71" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C71" s="21"/>
-      <c r="D71" s="21"/>
+      <c r="C71" s="27"/>
+      <c r="D71" s="27"/>
     </row>
     <row r="72" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C72" s="21"/>
-      <c r="D72" s="21"/>
+      <c r="C72" s="27"/>
+      <c r="D72" s="27"/>
     </row>
     <row r="73" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C73" s="21"/>
-      <c r="D73" s="21"/>
+      <c r="C73" s="27"/>
+      <c r="D73" s="27"/>
     </row>
     <row r="74" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C74" s="21"/>
-      <c r="D74" s="21"/>
+      <c r="C74" s="27"/>
+      <c r="D74" s="27"/>
     </row>
     <row r="75" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C75" s="21"/>
-      <c r="D75" s="21"/>
+      <c r="C75" s="27"/>
+      <c r="D75" s="27"/>
     </row>
     <row r="76" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C76" s="21"/>
-      <c r="D76" s="21"/>
+      <c r="C76" s="27"/>
+      <c r="D76" s="27"/>
     </row>
     <row r="77" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C77" s="21"/>
-      <c r="D77" s="21"/>
+      <c r="C77" s="27"/>
+      <c r="D77" s="27"/>
     </row>
     <row r="78" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C78" s="21"/>
-      <c r="D78" s="21"/>
+      <c r="C78" s="27"/>
+      <c r="D78" s="27"/>
     </row>
     <row r="79" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C79" s="21"/>
-      <c r="D79" s="21"/>
+      <c r="C79" s="27"/>
+      <c r="D79" s="27"/>
     </row>
     <row r="80" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C80" s="21"/>
-      <c r="D80" s="21"/>
+      <c r="C80" s="27"/>
+      <c r="D80" s="27"/>
     </row>
     <row r="81" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C81" s="21"/>
-      <c r="D81" s="21"/>
+      <c r="C81" s="27"/>
+      <c r="D81" s="27"/>
     </row>
     <row r="82" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C82" s="21"/>
-      <c r="D82" s="21"/>
+      <c r="C82" s="27"/>
+      <c r="D82" s="27"/>
     </row>
     <row r="83" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C83" s="21"/>
-      <c r="D83" s="21"/>
+      <c r="C83" s="27"/>
+      <c r="D83" s="27"/>
     </row>
     <row r="84" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C84" s="21"/>
-      <c r="D84" s="21"/>
+      <c r="C84" s="27"/>
+      <c r="D84" s="27"/>
     </row>
     <row r="85" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C85" s="21"/>
-      <c r="D85" s="21"/>
+      <c r="C85" s="27"/>
+      <c r="D85" s="27"/>
     </row>
     <row r="86" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C86" s="21"/>
-      <c r="D86" s="21"/>
+      <c r="C86" s="27"/>
+      <c r="D86" s="27"/>
     </row>
     <row r="87" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C87" s="21"/>
-      <c r="D87" s="21"/>
+      <c r="C87" s="27"/>
+      <c r="D87" s="27"/>
     </row>
     <row r="88" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C88" s="21"/>
-      <c r="D88" s="21"/>
+      <c r="C88" s="27"/>
+      <c r="D88" s="27"/>
     </row>
     <row r="89" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C89" s="21"/>
-      <c r="D89" s="21"/>
+      <c r="C89" s="27"/>
+      <c r="D89" s="27"/>
     </row>
     <row r="90" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C90" s="21"/>
-      <c r="D90" s="21"/>
+      <c r="C90" s="27"/>
+      <c r="D90" s="27"/>
     </row>
     <row r="91" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C91" s="21"/>
-      <c r="D91" s="21"/>
+      <c r="C91" s="27"/>
+      <c r="D91" s="27"/>
     </row>
     <row r="92" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C92" s="21"/>
-      <c r="D92" s="21"/>
+      <c r="C92" s="27"/>
+      <c r="D92" s="27"/>
     </row>
     <row r="93" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C93" s="21"/>
-      <c r="D93" s="21"/>
+      <c r="C93" s="27"/>
+      <c r="D93" s="27"/>
     </row>
     <row r="94" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C94" s="21"/>
-      <c r="D94" s="21"/>
+      <c r="C94" s="27"/>
+      <c r="D94" s="27"/>
     </row>
     <row r="95" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C95" s="21"/>
-      <c r="D95" s="21"/>
+      <c r="C95" s="27"/>
+      <c r="D95" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="84">
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C81:D81"/>
     <mergeCell ref="C94:D94"/>
     <mergeCell ref="C95:D95"/>
     <mergeCell ref="C10:D10"/>
@@ -3951,6 +3883,74 @@
     <mergeCell ref="C86:D86"/>
     <mergeCell ref="C87:D87"/>
     <mergeCell ref="C76:D76"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
   </mergeCells>
   <conditionalFormatting sqref="C2">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">

</xml_diff>

<commit_message>
Rename essential -> core, opportunity -> elective and other minor org changes
</commit_message>
<xml_diff>
--- a/rcc-ministry-catalog/src/main/resources/RCC Ministry Catalog.xlsx
+++ b/rcc-ministry-catalog/src/main/resources/RCC Ministry Catalog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20460" yWindow="0" windowWidth="7860" windowHeight="8565"/>
+    <workbookView xWindow="40920" yWindow="0" windowWidth="7860" windowHeight="8565"/>
   </bookViews>
   <sheets>
     <sheet name="Outline" sheetId="5" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="238">
   <si>
     <t>Ministry Role:</t>
   </si>
@@ -260,9 +260,6 @@
     <t>Admin &amp; Logistics</t>
   </si>
   <si>
-    <t>Website</t>
-  </si>
-  <si>
     <t>1.1.1</t>
   </si>
   <si>
@@ -299,9 +296,6 @@
     <t>Office Supplies</t>
   </si>
   <si>
-    <t>1.2.1</t>
-  </si>
-  <si>
     <t>1.2.2</t>
   </si>
   <si>
@@ -323,436 +317,436 @@
     <t>Budget</t>
   </si>
   <si>
+    <t>Tithe Counting</t>
+  </si>
+  <si>
+    <t>Building Committee</t>
+  </si>
+  <si>
+    <t>Elizabeth Elder</t>
+  </si>
+  <si>
+    <t>1.4.1</t>
+  </si>
+  <si>
+    <t>Capital Campaign</t>
+  </si>
+  <si>
+    <t>Property &amp; Building Maintenance</t>
+  </si>
+  <si>
+    <t>Aesthetics Committee</t>
+  </si>
+  <si>
+    <t>Celebration &amp; Fellowship</t>
+  </si>
+  <si>
+    <t>Celebration Events</t>
+  </si>
+  <si>
+    <t>2.1.1</t>
+  </si>
+  <si>
+    <t>Christmas Eve Service</t>
+  </si>
+  <si>
+    <t>2.1.2</t>
+  </si>
+  <si>
+    <t>Easter/Palm Sunday/Seder</t>
+  </si>
+  <si>
+    <t>2.1.3</t>
+  </si>
+  <si>
+    <t>Baptism</t>
+  </si>
+  <si>
+    <t>2.1.4</t>
+  </si>
+  <si>
+    <t>Lord's Supper</t>
+  </si>
+  <si>
+    <t>Fellowship</t>
+  </si>
+  <si>
+    <t>2.2.1</t>
+  </si>
+  <si>
+    <t>2.2.2</t>
+  </si>
+  <si>
+    <t>Potlucks</t>
+  </si>
+  <si>
+    <t>Welcoming</t>
+  </si>
+  <si>
+    <t>2.3.1</t>
+  </si>
+  <si>
+    <t>2.3.2</t>
+  </si>
+  <si>
+    <t>Site Utilization</t>
+  </si>
+  <si>
+    <t>Christian Education</t>
+  </si>
+  <si>
+    <t>Adult Sunday School</t>
+  </si>
+  <si>
+    <t>Bob Booth</t>
+  </si>
+  <si>
+    <t>Todd Harrell</t>
+  </si>
+  <si>
+    <t>Child Sunday School</t>
+  </si>
+  <si>
+    <t>3.2.1</t>
+  </si>
+  <si>
+    <t>Nursery</t>
+  </si>
+  <si>
+    <t>3.2.2</t>
+  </si>
+  <si>
+    <t>Preschool</t>
+  </si>
+  <si>
+    <t>3.2.3</t>
+  </si>
+  <si>
+    <t>Elementary</t>
+  </si>
+  <si>
+    <t>3.2.4</t>
+  </si>
+  <si>
+    <t>Middle School</t>
+  </si>
+  <si>
+    <t>3.2.5</t>
+  </si>
+  <si>
+    <t>Sermon-Time</t>
+  </si>
+  <si>
+    <t>3.2.6</t>
+  </si>
+  <si>
+    <t>Teacher Training</t>
+  </si>
+  <si>
+    <t>High School</t>
+  </si>
+  <si>
+    <t>3.3.1</t>
+  </si>
+  <si>
+    <t>3.3.2</t>
+  </si>
+  <si>
+    <t>High School Sunday School</t>
+  </si>
+  <si>
+    <t>New Members</t>
+  </si>
+  <si>
+    <t>3.4.1</t>
+  </si>
+  <si>
+    <t>New Members Class</t>
+  </si>
+  <si>
+    <t>3.4.2</t>
+  </si>
+  <si>
+    <t>New Members Fellowship</t>
+  </si>
+  <si>
+    <t>High School Fellowship</t>
+  </si>
+  <si>
+    <t>Tom Starkey</t>
+  </si>
+  <si>
+    <t>Local Missions</t>
+  </si>
+  <si>
+    <t>4.1.1</t>
+  </si>
+  <si>
+    <t>Pregnancy Centers of Central VA</t>
+  </si>
+  <si>
+    <t>4.1.2</t>
+  </si>
+  <si>
+    <t>International Students Inc.</t>
+  </si>
+  <si>
+    <t>4.1.3</t>
+  </si>
+  <si>
+    <t>YoungLife</t>
+  </si>
+  <si>
+    <t>4.1.4</t>
+  </si>
+  <si>
+    <t>Center for Christian Study</t>
+  </si>
+  <si>
+    <t>International Missions</t>
+  </si>
+  <si>
+    <t>4.2.1</t>
+  </si>
+  <si>
+    <t>Betel</t>
+  </si>
+  <si>
+    <t>4.2.2</t>
+  </si>
+  <si>
+    <t>Haiti</t>
+  </si>
+  <si>
+    <t>Worship Team</t>
+  </si>
+  <si>
+    <t>5.1.1</t>
+  </si>
+  <si>
+    <t>Worship Band</t>
+  </si>
+  <si>
+    <t>5.1.2</t>
+  </si>
+  <si>
+    <t>Worship Leader Training</t>
+  </si>
+  <si>
+    <t>5.2.1</t>
+  </si>
+  <si>
+    <t>5.2.2</t>
+  </si>
+  <si>
+    <t>5.2.3</t>
+  </si>
+  <si>
+    <t>Sermon Recording &amp; Uploading</t>
+  </si>
+  <si>
+    <t>Worship Audio/Video</t>
+  </si>
+  <si>
+    <t>Lyrics Projection</t>
+  </si>
+  <si>
+    <t>Home Groups</t>
+  </si>
+  <si>
+    <t>Home Group Leadership</t>
+  </si>
+  <si>
+    <t>6.2.1</t>
+  </si>
+  <si>
+    <t>Home Group Leaders Meetings</t>
+  </si>
+  <si>
+    <t>6.2.2</t>
+  </si>
+  <si>
+    <t>Home Group Leaders</t>
+  </si>
+  <si>
+    <t>6.2.3</t>
+  </si>
+  <si>
+    <t>Home Group Assistant Leaders</t>
+  </si>
+  <si>
+    <t>Home Group Ministry</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>Pre-service Prayer</t>
+  </si>
+  <si>
+    <t>Post-service Prayer</t>
+  </si>
+  <si>
+    <t>Jennifer Knight</t>
+  </si>
+  <si>
+    <t>Camping</t>
+  </si>
+  <si>
+    <t>Women's/Men's Fellowship</t>
+  </si>
+  <si>
+    <t>Marketing &amp; Advertising</t>
+  </si>
+  <si>
+    <t>Library</t>
+  </si>
+  <si>
+    <t>2.3.3</t>
+  </si>
+  <si>
+    <t>Visitor Welcoming</t>
+  </si>
+  <si>
+    <t>Visitor Follow-up</t>
+  </si>
+  <si>
+    <t>Youth Worship Band</t>
+  </si>
+  <si>
+    <t>5.1.3</t>
+  </si>
+  <si>
+    <t>Barbara Greb</t>
+  </si>
+  <si>
+    <t>Prayer Training</t>
+  </si>
+  <si>
+    <t>Prayer Retreats</t>
+  </si>
+  <si>
+    <t>Head/POC 1</t>
+  </si>
+  <si>
+    <t>Head/POC 2</t>
+  </si>
+  <si>
+    <t>Lisa Murray</t>
+  </si>
+  <si>
+    <t>Jerry King</t>
+  </si>
+  <si>
+    <t>Leigh Ann Skipper</t>
+  </si>
+  <si>
+    <t>John Dimeo</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>j.a.dimeo@gmail.com</t>
+  </si>
+  <si>
+    <t>434-964-0325</t>
+  </si>
+  <si>
+    <t>2bgreb@gmail.com</t>
+  </si>
+  <si>
+    <t>laskippy23@gmail.com</t>
+  </si>
+  <si>
+    <t>sknightrivanna@gmail.com</t>
+  </si>
+  <si>
+    <t>rivannachurch@gmail.com</t>
+  </si>
+  <si>
+    <t>434-975-0011</t>
+  </si>
+  <si>
+    <t>hoodgang0@gmail.com</t>
+  </si>
+  <si>
+    <t>tomstarkey01@gmail.com</t>
+  </si>
+  <si>
+    <t>elder.beth@gmail.com</t>
+  </si>
+  <si>
+    <t>rll9e@virginia.edu</t>
+  </si>
+  <si>
+    <t>harrelltm@yahoo.com</t>
+  </si>
+  <si>
+    <t>lamkem@yahoo.com</t>
+  </si>
+  <si>
+    <t>bboothjr93@gmail.com</t>
+  </si>
+  <si>
+    <t>Head/POC 3</t>
+  </si>
+  <si>
+    <t>Ministry Types</t>
+  </si>
+  <si>
+    <t>Interpretation</t>
+  </si>
+  <si>
+    <t>Gift 1</t>
+  </si>
+  <si>
+    <t>Gift 2</t>
+  </si>
+  <si>
+    <t>Gift 3</t>
+  </si>
+  <si>
+    <t>New Building</t>
+  </si>
+  <si>
+    <t>1.4.2</t>
+  </si>
+  <si>
+    <t>Kevin Murray</t>
+  </si>
+  <si>
+    <t>Core</t>
+  </si>
+  <si>
+    <t>Elective</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>1.1.3</t>
+  </si>
+  <si>
     <t>1.3.2</t>
   </si>
   <si>
-    <t>Tithe Counting</t>
-  </si>
-  <si>
-    <t>Building Committee</t>
-  </si>
-  <si>
-    <t>Elizabeth Elder</t>
-  </si>
-  <si>
-    <t>1.4.1</t>
-  </si>
-  <si>
-    <t>Capital Campaign</t>
-  </si>
-  <si>
-    <t>Property &amp; Building Maintenance</t>
-  </si>
-  <si>
-    <t>Aesthetics Committee</t>
-  </si>
-  <si>
-    <t>Celebration &amp; Fellowship</t>
-  </si>
-  <si>
-    <t>Celebration Events</t>
-  </si>
-  <si>
-    <t>2.1.1</t>
-  </si>
-  <si>
-    <t>Christmas Eve Service</t>
-  </si>
-  <si>
-    <t>2.1.2</t>
-  </si>
-  <si>
-    <t>Easter/Palm Sunday/Seder</t>
-  </si>
-  <si>
-    <t>2.1.3</t>
-  </si>
-  <si>
-    <t>Baptism</t>
-  </si>
-  <si>
-    <t>2.1.4</t>
-  </si>
-  <si>
-    <t>Lord's Supper</t>
-  </si>
-  <si>
-    <t>Fellowship</t>
-  </si>
-  <si>
-    <t>2.2.1</t>
-  </si>
-  <si>
-    <t>2.2.2</t>
-  </si>
-  <si>
-    <t>Potlucks</t>
-  </si>
-  <si>
-    <t>2.2.3</t>
-  </si>
-  <si>
-    <t>Fellowship Childcare</t>
-  </si>
-  <si>
-    <t>Welcoming</t>
-  </si>
-  <si>
-    <t>2.3.1</t>
-  </si>
-  <si>
-    <t>Ushers &amp; Greeters</t>
-  </si>
-  <si>
-    <t>2.3.2</t>
-  </si>
-  <si>
-    <t>Sunday Coffee</t>
-  </si>
-  <si>
-    <t>Site Utilization</t>
-  </si>
-  <si>
-    <t>Christian Education</t>
-  </si>
-  <si>
-    <t>Essential</t>
-  </si>
-  <si>
-    <t>Adult Sunday School</t>
-  </si>
-  <si>
-    <t>Bob Booth</t>
-  </si>
-  <si>
-    <t>Todd Harrell</t>
-  </si>
-  <si>
-    <t>Child Sunday School</t>
-  </si>
-  <si>
-    <t>3.2.1</t>
-  </si>
-  <si>
-    <t>Nursery</t>
-  </si>
-  <si>
-    <t>3.2.2</t>
-  </si>
-  <si>
-    <t>Preschool</t>
-  </si>
-  <si>
-    <t>3.2.3</t>
-  </si>
-  <si>
-    <t>Elementary</t>
-  </si>
-  <si>
-    <t>3.2.4</t>
-  </si>
-  <si>
-    <t>Middle School</t>
-  </si>
-  <si>
-    <t>3.2.5</t>
-  </si>
-  <si>
-    <t>Sermon-Time</t>
-  </si>
-  <si>
-    <t>3.2.6</t>
-  </si>
-  <si>
-    <t>Teacher Training</t>
-  </si>
-  <si>
-    <t>High School</t>
-  </si>
-  <si>
-    <t>3.3.1</t>
-  </si>
-  <si>
-    <t>3.3.2</t>
-  </si>
-  <si>
-    <t>High School Sunday School</t>
-  </si>
-  <si>
-    <t>New Members</t>
-  </si>
-  <si>
-    <t>3.4.1</t>
-  </si>
-  <si>
-    <t>New Members Class</t>
-  </si>
-  <si>
-    <t>3.4.2</t>
-  </si>
-  <si>
-    <t>New Members Fellowship</t>
-  </si>
-  <si>
-    <t>High School Fellowship</t>
-  </si>
-  <si>
-    <t>Tom Starkey</t>
-  </si>
-  <si>
-    <t>Local Missions</t>
-  </si>
-  <si>
-    <t>4.1.1</t>
-  </si>
-  <si>
-    <t>Pregnancy Centers of Central VA</t>
-  </si>
-  <si>
-    <t>4.1.2</t>
-  </si>
-  <si>
-    <t>International Students Inc.</t>
-  </si>
-  <si>
-    <t>4.1.3</t>
-  </si>
-  <si>
-    <t>YoungLife</t>
-  </si>
-  <si>
-    <t>4.1.4</t>
-  </si>
-  <si>
-    <t>Center for Christian Study</t>
-  </si>
-  <si>
-    <t>International Missions</t>
-  </si>
-  <si>
-    <t>4.2.1</t>
-  </si>
-  <si>
-    <t>Betel</t>
-  </si>
-  <si>
-    <t>4.2.2</t>
-  </si>
-  <si>
-    <t>Haiti</t>
-  </si>
-  <si>
-    <t>Worship Team</t>
-  </si>
-  <si>
-    <t>5.1.1</t>
-  </si>
-  <si>
-    <t>Worship Band</t>
-  </si>
-  <si>
-    <t>5.1.2</t>
-  </si>
-  <si>
-    <t>Worship Leader Training</t>
-  </si>
-  <si>
-    <t>5.2.1</t>
-  </si>
-  <si>
-    <t>5.2.2</t>
-  </si>
-  <si>
-    <t>5.2.3</t>
-  </si>
-  <si>
-    <t>Sermon Recording &amp; Uploading</t>
-  </si>
-  <si>
-    <t>Worship Audio/Video</t>
-  </si>
-  <si>
-    <t>Lyrics Projection</t>
-  </si>
-  <si>
-    <t>Home Groups</t>
-  </si>
-  <si>
-    <t>Home Group Leadership</t>
-  </si>
-  <si>
-    <t>6.2.1</t>
-  </si>
-  <si>
-    <t>Home Group Leaders Meetings</t>
-  </si>
-  <si>
-    <t>6.2.2</t>
-  </si>
-  <si>
-    <t>Home Group Leaders</t>
-  </si>
-  <si>
-    <t>6.2.3</t>
-  </si>
-  <si>
-    <t>Home Group Assistant Leaders</t>
-  </si>
-  <si>
-    <t>Home Group Ministry</t>
-  </si>
-  <si>
-    <t>Media</t>
-  </si>
-  <si>
-    <t>Pre-service Prayer</t>
-  </si>
-  <si>
-    <t>Post-service Prayer</t>
-  </si>
-  <si>
-    <t>Jennifer Knight</t>
-  </si>
-  <si>
-    <t>2.2.4</t>
-  </si>
-  <si>
-    <t>Camping</t>
-  </si>
-  <si>
-    <t>Opportunity</t>
-  </si>
-  <si>
-    <t>2.2.5</t>
-  </si>
-  <si>
-    <t>Women's/Men's Fellowship</t>
-  </si>
-  <si>
-    <t>Marketing &amp; Advertising</t>
-  </si>
-  <si>
-    <t>Library</t>
-  </si>
-  <si>
-    <t>2.3.3</t>
-  </si>
-  <si>
-    <t>Visitor Welcoming</t>
-  </si>
-  <si>
-    <t>Visitor Follow-up</t>
-  </si>
-  <si>
-    <t>Youth Worship Band</t>
-  </si>
-  <si>
-    <t>5.1.3</t>
-  </si>
-  <si>
-    <t>Barbara Greb</t>
-  </si>
-  <si>
-    <t>Prayer Training</t>
-  </si>
-  <si>
-    <t>Prayer Retreats</t>
-  </si>
-  <si>
-    <t>Head/POC 1</t>
-  </si>
-  <si>
-    <t>Head/POC 2</t>
-  </si>
-  <si>
-    <t>Lisa Murray</t>
-  </si>
-  <si>
-    <t>Jerry King</t>
-  </si>
-  <si>
-    <t>Leigh Ann Skipper</t>
-  </si>
-  <si>
-    <t>John Dimeo</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>j.a.dimeo@gmail.com</t>
-  </si>
-  <si>
-    <t>434-964-0325</t>
-  </si>
-  <si>
-    <t>2bgreb@gmail.com</t>
-  </si>
-  <si>
-    <t>laskippy23@gmail.com</t>
-  </si>
-  <si>
-    <t>sknightrivanna@gmail.com</t>
-  </si>
-  <si>
-    <t>rivannachurch@gmail.com</t>
-  </si>
-  <si>
-    <t>434-975-0011</t>
-  </si>
-  <si>
-    <t>hoodgang0@gmail.com</t>
-  </si>
-  <si>
-    <t>tomstarkey01@gmail.com</t>
-  </si>
-  <si>
-    <t>elder.beth@gmail.com</t>
-  </si>
-  <si>
-    <t>rll9e@virginia.edu</t>
-  </si>
-  <si>
-    <t>harrelltm@yahoo.com</t>
-  </si>
-  <si>
-    <t>lamkem@yahoo.com</t>
-  </si>
-  <si>
-    <t>bboothjr93@gmail.com</t>
-  </si>
-  <si>
-    <t>Head/POC 3</t>
-  </si>
-  <si>
-    <t>Ministry Types</t>
-  </si>
-  <si>
-    <t>Interpretation</t>
-  </si>
-  <si>
-    <t>Gift 1</t>
-  </si>
-  <si>
-    <t>Gift 2</t>
-  </si>
-  <si>
-    <t>Gift 3</t>
-  </si>
-  <si>
-    <t>New Building</t>
-  </si>
-  <si>
-    <t>1.4.2</t>
-  </si>
-  <si>
-    <t>Kevin Murray</t>
+    <t>2.1.5</t>
+  </si>
+  <si>
+    <t>2.4.1</t>
+  </si>
+  <si>
+    <t>Sunday Service Setup</t>
+  </si>
+  <si>
+    <t>Greeters</t>
   </si>
 </sst>
 </file>
@@ -927,6 +921,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -945,21 +940,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1340,12 +1334,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L80"/>
+  <dimension ref="A1:L79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
-      <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
+      <selection pane="bottomLeft" activeCell="G46" sqref="G46:H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1373,28 +1367,28 @@
         <v>72</v>
       </c>
       <c r="E1" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="19" t="s">
-        <v>81</v>
-      </c>
       <c r="G1" s="19" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="I1" s="19" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1405,13 +1399,13 @@
         <v>74</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>127</v>
+        <v>229</v>
       </c>
       <c r="F2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" s="16" t="s">
         <v>82</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1419,18 +1413,18 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>231</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C4" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" t="s">
         <v>76</v>
-      </c>
-      <c r="D4" t="s">
-        <v>77</v>
       </c>
       <c r="J4" t="s">
         <v>44</v>
@@ -1444,10 +1438,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C5" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J5" t="s">
         <v>15</v>
@@ -1457,33 +1451,33 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="17">
-        <v>1.2</v>
+      <c r="C6" s="17" t="s">
+        <v>232</v>
       </c>
       <c r="D6" t="s">
         <v>84</v>
       </c>
-      <c r="G6" s="16" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C7" s="17" t="s">
-        <v>88</v>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="17">
+        <v>1.2</v>
       </c>
       <c r="D7" t="s">
-        <v>85</v>
-      </c>
-      <c r="J7" t="s">
-        <v>30</v>
+        <v>83</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C8" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J8" t="s">
         <v>15</v>
@@ -1491,10 +1485,10 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C9" s="17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J9" t="s">
         <v>29</v>
@@ -1508,18 +1502,18 @@
         <v>1.3</v>
       </c>
       <c r="D10" t="s">
-        <v>92</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C11" s="17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D11" t="s">
-        <v>95</v>
+        <v>93</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>91</v>
       </c>
       <c r="J11" t="s">
         <v>15</v>
@@ -1533,10 +1527,13 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C12" s="17" t="s">
-        <v>96</v>
+        <v>233</v>
       </c>
       <c r="D12" t="s">
-        <v>97</v>
+        <v>94</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>89</v>
       </c>
       <c r="J12" t="s">
         <v>15</v>
@@ -1550,18 +1547,18 @@
         <v>1.4</v>
       </c>
       <c r="D13" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C14" s="17" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D14" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="J14" t="s">
         <v>22</v>
@@ -1569,13 +1566,13 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C15" s="17" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="D15" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1583,523 +1580,541 @@
         <v>1.5</v>
       </c>
       <c r="D16" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B17" s="17">
         <v>1.6</v>
       </c>
       <c r="D17" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J17" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B18" s="17">
         <v>1.7</v>
       </c>
       <c r="D18" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+      <c r="J18" t="s">
+        <v>20</v>
+      </c>
+      <c r="K18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B19" s="17">
         <v>1.8</v>
       </c>
       <c r="D19" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="17">
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>127</v>
+        <v>229</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="H20" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B21" s="17">
         <v>2.1</v>
       </c>
       <c r="D21" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C22" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="D22" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C23" s="17" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C22" s="17" t="s">
+      <c r="D23" t="s">
         <v>106</v>
       </c>
-      <c r="D22" t="s">
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C24" s="17" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C23" s="17" t="s">
+      <c r="D24" t="s">
         <v>108</v>
       </c>
-      <c r="D23" t="s">
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C25" s="17" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C24" s="17" t="s">
+      <c r="D25" t="s">
         <v>110</v>
       </c>
-      <c r="D24" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C25" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="D25" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="17">
-        <v>2.2000000000000002</v>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C26" s="17" t="s">
+        <v>234</v>
       </c>
       <c r="D26" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C27" s="17" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="17">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D27" t="s">
+        <v>111</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C28" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="D28" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C29" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="D29" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="17">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D30" t="s">
         <v>115</v>
       </c>
-      <c r="D27" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C28" s="17" t="s">
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C31" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D31" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C32" s="17" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C29" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="D29" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C30" s="17" t="s">
-        <v>193</v>
-      </c>
-      <c r="D30" t="s">
-        <v>194</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C31" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D31" t="s">
-        <v>197</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="17">
-        <v>2.2999999999999998</v>
-      </c>
       <c r="D32" t="s">
-        <v>120</v>
+        <v>190</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C33" s="17" t="s">
-        <v>121</v>
+        <v>189</v>
       </c>
       <c r="D33" t="s">
-        <v>122</v>
+        <v>191</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C34" s="17" t="s">
-        <v>123</v>
+      <c r="B34" s="17">
+        <v>2.4</v>
       </c>
       <c r="D34" t="s">
-        <v>201</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C35" s="17" t="s">
-        <v>200</v>
+        <v>235</v>
       </c>
       <c r="D35" t="s">
-        <v>202</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>195</v>
+        <v>236</v>
+      </c>
+      <c r="G35" s="16" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="17">
-        <v>2.4</v>
+      <c r="A36" s="17">
+        <v>3</v>
       </c>
       <c r="D36" t="s">
-        <v>125</v>
+        <v>119</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="17">
-        <v>3</v>
+      <c r="B37" s="17">
+        <v>3.1</v>
       </c>
       <c r="D37" t="s">
-        <v>126</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
+      </c>
+      <c r="G37" s="16" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B38" s="17">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="D38" t="s">
-        <v>128</v>
-      </c>
-      <c r="G38" s="16" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="17">
-        <v>3.2</v>
+      <c r="C39" s="17" t="s">
+        <v>124</v>
       </c>
       <c r="D39" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C40" s="17" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D40" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C41" s="17" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D41" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C42" s="17" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D42" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C43" s="17" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D43" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C44" s="17" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D44" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C45" s="17" t="s">
-        <v>142</v>
+      <c r="B45" s="17">
+        <v>3.3</v>
       </c>
       <c r="D45" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="17">
-        <v>3.3</v>
+      <c r="C46" s="17" t="s">
+        <v>137</v>
       </c>
       <c r="D46" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G46" s="16" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="H46" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C47" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="D47" t="s">
         <v>145</v>
       </c>
-      <c r="D47" t="s">
-        <v>147</v>
+      <c r="E47" s="1" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C48" s="17" t="s">
-        <v>146</v>
+      <c r="B48" s="17">
+        <v>3.4</v>
       </c>
       <c r="D48" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B49" s="17">
-        <v>3.4</v>
+      <c r="C49" s="17" t="s">
+        <v>141</v>
       </c>
       <c r="D49" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C50" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="D50" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="17">
+        <v>4</v>
+      </c>
+      <c r="D51" t="s">
+        <v>71</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F51" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B52" s="17">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D52" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C53" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D53" t="s">
         <v>149</v>
-      </c>
-      <c r="D50" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C51" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="D51" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" s="17">
-        <v>4</v>
-      </c>
-      <c r="D52" t="s">
-        <v>71</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F52" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B53" s="17">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="D53" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C54" s="17" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D54" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C55" s="17" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D55" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C56" s="17" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D56" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C57" s="17" t="s">
-        <v>162</v>
+      <c r="B57" s="17">
+        <v>4.2</v>
       </c>
       <c r="D57" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B58" s="17">
-        <v>4.2</v>
+      <c r="C58" s="17" t="s">
+        <v>157</v>
       </c>
       <c r="D58" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C59" s="17" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D59" t="s">
-        <v>166</v>
+        <v>160</v>
+      </c>
+      <c r="J59" t="s">
+        <v>16</v>
+      </c>
+      <c r="K59" t="s">
+        <v>37</v>
+      </c>
+      <c r="L59" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C60" s="17" t="s">
-        <v>167</v>
+      <c r="A60" s="17">
+        <v>5</v>
       </c>
       <c r="D60" t="s">
-        <v>168</v>
-      </c>
-      <c r="J60" t="s">
-        <v>16</v>
-      </c>
-      <c r="K60" t="s">
-        <v>37</v>
-      </c>
-      <c r="L60" t="s">
-        <v>42</v>
+        <v>161</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F60" t="s">
+        <v>81</v>
+      </c>
+      <c r="G60" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="H60" t="s">
+        <v>201</v>
+      </c>
+      <c r="I60" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A61" s="17">
-        <v>5</v>
+      <c r="B61" s="17">
+        <v>5.0999999999999996</v>
       </c>
       <c r="D61" t="s">
-        <v>169</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F61" t="s">
-        <v>82</v>
-      </c>
-      <c r="G61" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="H61" t="s">
-        <v>212</v>
-      </c>
-      <c r="I61" t="s">
-        <v>213</v>
+        <v>43</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B62" s="17">
-        <v>5.0999999999999996</v>
+      <c r="C62" s="17" t="s">
+        <v>162</v>
       </c>
       <c r="D62" t="s">
+        <v>163</v>
+      </c>
+      <c r="J62" t="s">
         <v>43</v>
+      </c>
+      <c r="K62" t="s">
+        <v>21</v>
+      </c>
+      <c r="L62" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C63" s="17" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="D63" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="J63" t="s">
         <v>43</v>
       </c>
       <c r="K63" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="L63" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C64" s="17" t="s">
-        <v>172</v>
+        <v>193</v>
       </c>
       <c r="D64" t="s">
-        <v>173</v>
+        <v>192</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="G64" s="16" t="s">
+        <v>194</v>
       </c>
       <c r="J64" t="s">
         <v>43</v>
       </c>
       <c r="K64" t="s">
-        <v>35</v>
-      </c>
-      <c r="L64" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B65" s="17">
+        <v>5.2</v>
+      </c>
+      <c r="D65" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C66" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="D66" t="s">
+        <v>170</v>
+      </c>
+      <c r="J66" t="s">
+        <v>44</v>
+      </c>
+      <c r="K66" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C65" s="17" t="s">
-        <v>204</v>
-      </c>
-      <c r="D65" t="s">
-        <v>203</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="G65" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="J65" t="s">
+      <c r="L66" t="s">
         <v>43</v>
-      </c>
-      <c r="K65" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B66" s="17">
-        <v>5.2</v>
-      </c>
-      <c r="D66" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C67" s="17" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="D67" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="J67" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="K67" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="L67" t="s">
         <v>43</v>
@@ -2107,10 +2122,10 @@
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C68" s="17" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="D68" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="J68" t="s">
         <v>15</v>
@@ -2123,182 +2138,165 @@
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C69" s="17" t="s">
-        <v>176</v>
+      <c r="A69" s="17">
+        <v>6</v>
       </c>
       <c r="D69" t="s">
-        <v>179</v>
-      </c>
-      <c r="J69" t="s">
-        <v>15</v>
-      </c>
-      <c r="K69" t="s">
-        <v>42</v>
-      </c>
-      <c r="L69" t="s">
-        <v>43</v>
+        <v>180</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A70" s="17">
-        <v>6</v>
+      <c r="B70" s="17">
+        <v>6.1</v>
       </c>
       <c r="D70" t="s">
-        <v>188</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>127</v>
+        <v>172</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B71" s="17">
-        <v>6.1</v>
+        <v>6.2</v>
       </c>
       <c r="D71" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B72" s="17">
-        <v>6.2</v>
+      <c r="C72" s="17" t="s">
+        <v>174</v>
       </c>
       <c r="D72" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C73" s="17" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D73" t="s">
-        <v>183</v>
+        <v>177</v>
+      </c>
+      <c r="J73" t="s">
+        <v>20</v>
+      </c>
+      <c r="K73" t="s">
+        <v>31</v>
+      </c>
+      <c r="L73" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C74" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D74" t="s">
+        <v>179</v>
+      </c>
+      <c r="J74" t="s">
+        <v>15</v>
+      </c>
+      <c r="K74" t="s">
+        <v>34</v>
+      </c>
+      <c r="L74" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A75" s="17">
+        <v>7</v>
+      </c>
+      <c r="D75" t="s">
+        <v>32</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="G75" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="D74" t="s">
-        <v>185</v>
-      </c>
-      <c r="J74" t="s">
-        <v>20</v>
-      </c>
-      <c r="K74" t="s">
-        <v>31</v>
-      </c>
-      <c r="L74" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C75" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="D75" t="s">
-        <v>187</v>
-      </c>
-      <c r="J75" t="s">
-        <v>15</v>
-      </c>
-      <c r="K75" t="s">
-        <v>34</v>
-      </c>
-      <c r="L75" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A76" s="17">
-        <v>7</v>
+      <c r="B76" s="17">
+        <v>7.1</v>
       </c>
       <c r="D76" t="s">
+        <v>182</v>
+      </c>
+      <c r="J76" t="s">
         <v>32</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="G76" s="16" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B77" s="17">
-        <v>7.1</v>
+        <v>7.2</v>
       </c>
       <c r="D77" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="J77" t="s">
         <v>32</v>
       </c>
+      <c r="K77" t="s">
+        <v>41</v>
+      </c>
+      <c r="L77" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B78" s="17">
-        <v>7.2</v>
+        <v>7.3</v>
       </c>
       <c r="D78" t="s">
-        <v>191</v>
+        <v>195</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>230</v>
       </c>
       <c r="J78" t="s">
         <v>32</v>
       </c>
       <c r="K78" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L78" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B79" s="17">
-        <v>7.3</v>
+        <v>7.4</v>
       </c>
       <c r="D79" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>195</v>
+        <v>230</v>
       </c>
       <c r="J79" t="s">
         <v>32</v>
       </c>
       <c r="K79" t="s">
+        <v>15</v>
+      </c>
+      <c r="L79" t="s">
         <v>35</v>
       </c>
-      <c r="L79" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B80" s="17">
-        <v>7.4</v>
-      </c>
-      <c r="D80" t="s">
-        <v>207</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="J80" t="s">
-        <v>32</v>
-      </c>
-      <c r="K80" t="s">
-        <v>15</v>
-      </c>
-      <c r="L80" t="s">
-        <v>35</v>
-      </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Not in directory" error="You have entered a person who is not in the Directory tab" sqref="G2:I201">
+  <dataValidations disablePrompts="1" count="3">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Not in directory" error="You have entered a person who is not in the Directory tab" sqref="G2:I9 H10:I27 G11:G27 I28:I200 G46:H200 G28:H44">
       <formula1>INDIRECT("TDirectory[Name]")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E221">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E220">
       <formula1>INDIRECT("TMinistryTypes[Ministry Types]")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:L201">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:L200">
       <formula1>INDIRECT("TGifts[Gifts]")</formula1>
     </dataValidation>
   </dataValidations>
@@ -2324,123 +2322,123 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="B1" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="C1" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B5" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="C5" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="C7" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B12" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -2461,7 +2459,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2472,7 +2470,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="C1" t="s">
         <v>46</v>
@@ -2480,7 +2478,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>127</v>
+        <v>229</v>
       </c>
       <c r="C2" t="s">
         <v>39</v>
@@ -2488,7 +2486,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>195</v>
+        <v>230</v>
       </c>
       <c r="C3" t="s">
         <v>44</v>
@@ -2546,7 +2544,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2665,10 +2663,10 @@
         <f>Reference!A1</f>
         <v>Ministry Role:</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="23"/>
+      <c r="D1" s="24"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2685,10 +2683,10 @@
         <f>Reference!A3</f>
         <v>Filled by:</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="25"/>
+      <c r="D3" s="26"/>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2699,11 +2697,11 @@
         <f>Reference!A5</f>
         <v>In Ministry Area:</v>
       </c>
-      <c r="C5" s="26" t="e">
+      <c r="C5" s="27" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="D5" s="26"/>
+      <c r="D5" s="27"/>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2711,11 +2709,11 @@
         <f>Reference!A6</f>
         <v>Under Ministry Role:</v>
       </c>
-      <c r="C6" s="26" t="e">
+      <c r="C6" s="27" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="D6" s="26"/>
+      <c r="D6" s="27"/>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2746,10 +2744,10 @@
         <f>Reference!A10</f>
         <v>Position open to:</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="D10" s="25"/>
+      <c r="D10" s="26"/>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" ht="8.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2758,31 +2756,31 @@
         <f>Reference!A12</f>
         <v>Relevant gifts:</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="22"/>
+      <c r="D12" s="23"/>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="22"/>
+      <c r="D13" s="23"/>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="22"/>
+      <c r="D14" s="23"/>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="22"/>
+      <c r="D15" s="23"/>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2796,32 +2794,32 @@
         <f>Reference!A19</f>
         <v>Relevant skills:</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="22"/>
+      <c r="D17" s="23"/>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="22"/>
+      <c r="D18" s="23"/>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="D19" s="22"/>
+      <c r="D19" s="23"/>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="D20" s="22"/>
+      <c r="D20" s="23"/>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2835,24 +2833,24 @@
         <f>Reference!A25</f>
         <v>Personality:</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="D22" s="22"/>
+      <c r="D22" s="23"/>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="21" t="s">
+      <c r="C23" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="22"/>
+      <c r="D23" s="23"/>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="21" t="s">
+      <c r="C24" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="D24" s="22"/>
+      <c r="D24" s="23"/>
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2865,10 +2863,10 @@
         <f>Reference!A31</f>
         <v>Length of service:</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C26" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="D26" s="22"/>
+      <c r="D26" s="23"/>
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -2876,17 +2874,17 @@
         <f>Reference!A32</f>
         <v>Time commitments:</v>
       </c>
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="D27" s="22"/>
+      <c r="D27" s="23"/>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C28" s="21" t="s">
+      <c r="C28" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="22"/>
+      <c r="D28" s="23"/>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2899,246 +2897,309 @@
         <f>Reference!A38</f>
         <v>Responsibilities:</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C30" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="D30" s="22"/>
+      <c r="D30" s="23"/>
       <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C31" s="21" t="s">
+      <c r="C31" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="D31" s="22"/>
+      <c r="D31" s="23"/>
       <c r="E31" s="5"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C32" s="21" t="s">
+      <c r="C32" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="D32" s="22"/>
+      <c r="D32" s="23"/>
       <c r="E32" s="5"/>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C33" s="21" t="s">
+      <c r="C33" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="D33" s="22"/>
+      <c r="D33" s="23"/>
       <c r="E33" s="5"/>
     </row>
     <row r="34" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C34" s="21" t="s">
+      <c r="C34" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="D34" s="22"/>
+      <c r="D34" s="23"/>
       <c r="E34" s="5"/>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
     </row>
     <row r="36" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C36" s="27"/>
-      <c r="D36" s="27"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C37" s="27"/>
-      <c r="D37" s="27"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C38" s="27"/>
-      <c r="D38" s="27"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C39" s="27"/>
-      <c r="D39" s="27"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
     </row>
     <row r="40" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C40" s="27"/>
-      <c r="D40" s="27"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C41" s="27"/>
-      <c r="D41" s="27"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
     </row>
     <row r="42" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C42" s="27"/>
-      <c r="D42" s="27"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
     </row>
     <row r="43" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C43" s="27"/>
-      <c r="D43" s="27"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="21"/>
     </row>
     <row r="44" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C44" s="27"/>
-      <c r="D44" s="27"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="21"/>
     </row>
     <row r="45" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C45" s="27"/>
-      <c r="D45" s="27"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
     </row>
     <row r="46" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C46" s="27"/>
-      <c r="D46" s="27"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
     </row>
     <row r="47" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="21"/>
     </row>
     <row r="48" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C48" s="27"/>
-      <c r="D48" s="27"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="21"/>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C49" s="27"/>
-      <c r="D49" s="27"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C50" s="27"/>
-      <c r="D50" s="27"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="21"/>
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C51" s="27"/>
-      <c r="D51" s="27"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="21"/>
     </row>
     <row r="52" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C52" s="27"/>
-      <c r="D52" s="27"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="21"/>
     </row>
     <row r="53" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C53" s="27"/>
-      <c r="D53" s="27"/>
+      <c r="C53" s="21"/>
+      <c r="D53" s="21"/>
     </row>
     <row r="54" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C54" s="27"/>
-      <c r="D54" s="27"/>
+      <c r="C54" s="21"/>
+      <c r="D54" s="21"/>
     </row>
     <row r="55" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C55" s="27"/>
-      <c r="D55" s="27"/>
+      <c r="C55" s="21"/>
+      <c r="D55" s="21"/>
     </row>
     <row r="56" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C56" s="27"/>
-      <c r="D56" s="27"/>
+      <c r="C56" s="21"/>
+      <c r="D56" s="21"/>
     </row>
     <row r="57" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C57" s="27"/>
-      <c r="D57" s="27"/>
+      <c r="C57" s="21"/>
+      <c r="D57" s="21"/>
     </row>
     <row r="58" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C58" s="27"/>
-      <c r="D58" s="27"/>
+      <c r="C58" s="21"/>
+      <c r="D58" s="21"/>
     </row>
     <row r="59" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C59" s="27"/>
-      <c r="D59" s="27"/>
+      <c r="C59" s="21"/>
+      <c r="D59" s="21"/>
     </row>
     <row r="60" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C60" s="27"/>
-      <c r="D60" s="27"/>
+      <c r="C60" s="21"/>
+      <c r="D60" s="21"/>
     </row>
     <row r="61" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C61" s="27"/>
-      <c r="D61" s="27"/>
+      <c r="C61" s="21"/>
+      <c r="D61" s="21"/>
     </row>
     <row r="62" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C62" s="27"/>
-      <c r="D62" s="27"/>
+      <c r="C62" s="21"/>
+      <c r="D62" s="21"/>
     </row>
     <row r="63" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C63" s="27"/>
-      <c r="D63" s="27"/>
+      <c r="C63" s="21"/>
+      <c r="D63" s="21"/>
     </row>
     <row r="64" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C64" s="27"/>
-      <c r="D64" s="27"/>
+      <c r="C64" s="21"/>
+      <c r="D64" s="21"/>
     </row>
     <row r="65" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C65" s="27"/>
-      <c r="D65" s="27"/>
+      <c r="C65" s="21"/>
+      <c r="D65" s="21"/>
     </row>
     <row r="66" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C66" s="27"/>
-      <c r="D66" s="27"/>
+      <c r="C66" s="21"/>
+      <c r="D66" s="21"/>
     </row>
     <row r="67" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C67" s="27"/>
-      <c r="D67" s="27"/>
+      <c r="C67" s="21"/>
+      <c r="D67" s="21"/>
     </row>
     <row r="68" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C68" s="27"/>
-      <c r="D68" s="27"/>
+      <c r="C68" s="21"/>
+      <c r="D68" s="21"/>
     </row>
     <row r="69" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C69" s="27"/>
-      <c r="D69" s="27"/>
+      <c r="C69" s="21"/>
+      <c r="D69" s="21"/>
     </row>
     <row r="70" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C70" s="27"/>
-      <c r="D70" s="27"/>
+      <c r="C70" s="21"/>
+      <c r="D70" s="21"/>
     </row>
     <row r="71" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C71" s="27"/>
-      <c r="D71" s="27"/>
+      <c r="C71" s="21"/>
+      <c r="D71" s="21"/>
     </row>
     <row r="72" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C72" s="27"/>
-      <c r="D72" s="27"/>
+      <c r="C72" s="21"/>
+      <c r="D72" s="21"/>
     </row>
     <row r="73" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C73" s="27"/>
-      <c r="D73" s="27"/>
+      <c r="C73" s="21"/>
+      <c r="D73" s="21"/>
     </row>
     <row r="74" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C74" s="27"/>
-      <c r="D74" s="27"/>
+      <c r="C74" s="21"/>
+      <c r="D74" s="21"/>
     </row>
     <row r="75" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C75" s="27"/>
-      <c r="D75" s="27"/>
+      <c r="C75" s="21"/>
+      <c r="D75" s="21"/>
     </row>
     <row r="76" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C76" s="27"/>
-      <c r="D76" s="27"/>
+      <c r="C76" s="21"/>
+      <c r="D76" s="21"/>
     </row>
     <row r="77" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C77" s="27"/>
-      <c r="D77" s="27"/>
+      <c r="C77" s="21"/>
+      <c r="D77" s="21"/>
     </row>
     <row r="78" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C78" s="27"/>
-      <c r="D78" s="27"/>
+      <c r="C78" s="21"/>
+      <c r="D78" s="21"/>
     </row>
     <row r="79" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C79" s="27"/>
-      <c r="D79" s="27"/>
+      <c r="C79" s="21"/>
+      <c r="D79" s="21"/>
     </row>
     <row r="80" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C80" s="27"/>
-      <c r="D80" s="27"/>
+      <c r="C80" s="21"/>
+      <c r="D80" s="21"/>
     </row>
     <row r="81" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C81" s="27"/>
-      <c r="D81" s="27"/>
+      <c r="C81" s="21"/>
+      <c r="D81" s="21"/>
     </row>
     <row r="82" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C82" s="27"/>
-      <c r="D82" s="27"/>
+      <c r="C82" s="21"/>
+      <c r="D82" s="21"/>
     </row>
     <row r="83" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C83" s="27"/>
-      <c r="D83" s="27"/>
+      <c r="C83" s="21"/>
+      <c r="D83" s="21"/>
     </row>
     <row r="84" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C84" s="27"/>
-      <c r="D84" s="27"/>
+      <c r="C84" s="21"/>
+      <c r="D84" s="21"/>
     </row>
     <row r="85" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C85" s="27"/>
-      <c r="D85" s="27"/>
+      <c r="C85" s="21"/>
+      <c r="D85" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="75">
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="C72:D72"/>
     <mergeCell ref="C85:D85"/>
     <mergeCell ref="C74:D74"/>
     <mergeCell ref="C75:D75"/>
@@ -3151,69 +3212,6 @@
     <mergeCell ref="C82:D82"/>
     <mergeCell ref="C83:D83"/>
     <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C10:D10"/>
   </mergeCells>
   <conditionalFormatting sqref="C2">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
@@ -3273,8 +3271,8 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
       <c r="E1" s="1"/>
       <c r="F1" t="s">
         <v>45</v>
@@ -3333,8 +3331,8 @@
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
       <c r="E5" s="2"/>
       <c r="G5" t="s">
         <v>29</v>
@@ -3344,8 +3342,8 @@
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
       <c r="E6" s="2"/>
       <c r="G6" t="s">
         <v>23</v>
@@ -3632,241 +3630,309 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
-      <c r="C39" s="32"/>
-      <c r="D39" s="33"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="31"/>
       <c r="E39" s="5"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C40" s="32"/>
-      <c r="D40" s="33"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="31"/>
       <c r="E40" s="5"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C41" s="32"/>
-      <c r="D41" s="33"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="31"/>
       <c r="E41" s="5"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C42" s="32"/>
-      <c r="D42" s="33"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="31"/>
       <c r="E42" s="5"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C43" s="32"/>
-      <c r="D43" s="33"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="31"/>
       <c r="E43" s="5"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C44" s="32"/>
-      <c r="D44" s="33"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="31"/>
       <c r="E44" s="5"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C45" s="27"/>
-      <c r="D45" s="27"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C46" s="27"/>
-      <c r="D46" s="27"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="21"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C48" s="27"/>
-      <c r="D48" s="27"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="21"/>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C49" s="27"/>
-      <c r="D49" s="27"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C50" s="27"/>
-      <c r="D50" s="27"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="21"/>
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C51" s="27"/>
-      <c r="D51" s="27"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="21"/>
     </row>
     <row r="52" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C52" s="27"/>
-      <c r="D52" s="27"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="21"/>
     </row>
     <row r="53" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C53" s="27"/>
-      <c r="D53" s="27"/>
+      <c r="C53" s="21"/>
+      <c r="D53" s="21"/>
     </row>
     <row r="54" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C54" s="27"/>
-      <c r="D54" s="27"/>
+      <c r="C54" s="21"/>
+      <c r="D54" s="21"/>
     </row>
     <row r="55" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C55" s="27"/>
-      <c r="D55" s="27"/>
+      <c r="C55" s="21"/>
+      <c r="D55" s="21"/>
     </row>
     <row r="56" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C56" s="27"/>
-      <c r="D56" s="27"/>
+      <c r="C56" s="21"/>
+      <c r="D56" s="21"/>
     </row>
     <row r="57" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C57" s="27"/>
-      <c r="D57" s="27"/>
+      <c r="C57" s="21"/>
+      <c r="D57" s="21"/>
     </row>
     <row r="58" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C58" s="27"/>
-      <c r="D58" s="27"/>
+      <c r="C58" s="21"/>
+      <c r="D58" s="21"/>
     </row>
     <row r="59" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C59" s="27"/>
-      <c r="D59" s="27"/>
+      <c r="C59" s="21"/>
+      <c r="D59" s="21"/>
     </row>
     <row r="60" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C60" s="27"/>
-      <c r="D60" s="27"/>
+      <c r="C60" s="21"/>
+      <c r="D60" s="21"/>
     </row>
     <row r="61" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C61" s="27"/>
-      <c r="D61" s="27"/>
+      <c r="C61" s="21"/>
+      <c r="D61" s="21"/>
     </row>
     <row r="62" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C62" s="27"/>
-      <c r="D62" s="27"/>
+      <c r="C62" s="21"/>
+      <c r="D62" s="21"/>
     </row>
     <row r="63" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C63" s="27"/>
-      <c r="D63" s="27"/>
+      <c r="C63" s="21"/>
+      <c r="D63" s="21"/>
     </row>
     <row r="64" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C64" s="27"/>
-      <c r="D64" s="27"/>
+      <c r="C64" s="21"/>
+      <c r="D64" s="21"/>
     </row>
     <row r="65" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C65" s="27"/>
-      <c r="D65" s="27"/>
+      <c r="C65" s="21"/>
+      <c r="D65" s="21"/>
     </row>
     <row r="66" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C66" s="27"/>
-      <c r="D66" s="27"/>
+      <c r="C66" s="21"/>
+      <c r="D66" s="21"/>
     </row>
     <row r="67" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C67" s="27"/>
-      <c r="D67" s="27"/>
+      <c r="C67" s="21"/>
+      <c r="D67" s="21"/>
     </row>
     <row r="68" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C68" s="27"/>
-      <c r="D68" s="27"/>
+      <c r="C68" s="21"/>
+      <c r="D68" s="21"/>
     </row>
     <row r="69" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C69" s="27"/>
-      <c r="D69" s="27"/>
+      <c r="C69" s="21"/>
+      <c r="D69" s="21"/>
     </row>
     <row r="70" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C70" s="27"/>
-      <c r="D70" s="27"/>
+      <c r="C70" s="21"/>
+      <c r="D70" s="21"/>
     </row>
     <row r="71" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C71" s="27"/>
-      <c r="D71" s="27"/>
+      <c r="C71" s="21"/>
+      <c r="D71" s="21"/>
     </row>
     <row r="72" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C72" s="27"/>
-      <c r="D72" s="27"/>
+      <c r="C72" s="21"/>
+      <c r="D72" s="21"/>
     </row>
     <row r="73" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C73" s="27"/>
-      <c r="D73" s="27"/>
+      <c r="C73" s="21"/>
+      <c r="D73" s="21"/>
     </row>
     <row r="74" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C74" s="27"/>
-      <c r="D74" s="27"/>
+      <c r="C74" s="21"/>
+      <c r="D74" s="21"/>
     </row>
     <row r="75" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C75" s="27"/>
-      <c r="D75" s="27"/>
+      <c r="C75" s="21"/>
+      <c r="D75" s="21"/>
     </row>
     <row r="76" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C76" s="27"/>
-      <c r="D76" s="27"/>
+      <c r="C76" s="21"/>
+      <c r="D76" s="21"/>
     </row>
     <row r="77" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C77" s="27"/>
-      <c r="D77" s="27"/>
+      <c r="C77" s="21"/>
+      <c r="D77" s="21"/>
     </row>
     <row r="78" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C78" s="27"/>
-      <c r="D78" s="27"/>
+      <c r="C78" s="21"/>
+      <c r="D78" s="21"/>
     </row>
     <row r="79" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C79" s="27"/>
-      <c r="D79" s="27"/>
+      <c r="C79" s="21"/>
+      <c r="D79" s="21"/>
     </row>
     <row r="80" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C80" s="27"/>
-      <c r="D80" s="27"/>
+      <c r="C80" s="21"/>
+      <c r="D80" s="21"/>
     </row>
     <row r="81" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C81" s="27"/>
-      <c r="D81" s="27"/>
+      <c r="C81" s="21"/>
+      <c r="D81" s="21"/>
     </row>
     <row r="82" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C82" s="27"/>
-      <c r="D82" s="27"/>
+      <c r="C82" s="21"/>
+      <c r="D82" s="21"/>
     </row>
     <row r="83" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C83" s="27"/>
-      <c r="D83" s="27"/>
+      <c r="C83" s="21"/>
+      <c r="D83" s="21"/>
     </row>
     <row r="84" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C84" s="27"/>
-      <c r="D84" s="27"/>
+      <c r="C84" s="21"/>
+      <c r="D84" s="21"/>
     </row>
     <row r="85" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C85" s="27"/>
-      <c r="D85" s="27"/>
+      <c r="C85" s="21"/>
+      <c r="D85" s="21"/>
     </row>
     <row r="86" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C86" s="27"/>
-      <c r="D86" s="27"/>
+      <c r="C86" s="21"/>
+      <c r="D86" s="21"/>
     </row>
     <row r="87" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C87" s="27"/>
-      <c r="D87" s="27"/>
+      <c r="C87" s="21"/>
+      <c r="D87" s="21"/>
     </row>
     <row r="88" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C88" s="27"/>
-      <c r="D88" s="27"/>
+      <c r="C88" s="21"/>
+      <c r="D88" s="21"/>
     </row>
     <row r="89" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C89" s="27"/>
-      <c r="D89" s="27"/>
+      <c r="C89" s="21"/>
+      <c r="D89" s="21"/>
     </row>
     <row r="90" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C90" s="27"/>
-      <c r="D90" s="27"/>
+      <c r="C90" s="21"/>
+      <c r="D90" s="21"/>
     </row>
     <row r="91" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C91" s="27"/>
-      <c r="D91" s="27"/>
+      <c r="C91" s="21"/>
+      <c r="D91" s="21"/>
     </row>
     <row r="92" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C92" s="27"/>
-      <c r="D92" s="27"/>
+      <c r="C92" s="21"/>
+      <c r="D92" s="21"/>
     </row>
     <row r="93" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C93" s="27"/>
-      <c r="D93" s="27"/>
+      <c r="C93" s="21"/>
+      <c r="D93" s="21"/>
     </row>
     <row r="94" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C94" s="27"/>
-      <c r="D94" s="27"/>
+      <c r="C94" s="21"/>
+      <c r="D94" s="21"/>
     </row>
     <row r="95" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C95" s="27"/>
-      <c r="D95" s="27"/>
+      <c r="C95" s="21"/>
+      <c r="D95" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="84">
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C81:D81"/>
     <mergeCell ref="C94:D94"/>
     <mergeCell ref="C95:D95"/>
     <mergeCell ref="C10:D10"/>
@@ -3883,74 +3949,6 @@
     <mergeCell ref="C86:D86"/>
     <mergeCell ref="C87:D87"/>
     <mergeCell ref="C76:D76"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
   </mergeCells>
   <conditionalFormatting sqref="C2">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">

</xml_diff>

<commit_message>
Updates to catalog based on CHT meeting with Scott 2/7/2017
</commit_message>
<xml_diff>
--- a/rcc-ministry-catalog/src/main/resources/RCC Ministry Catalog.xlsx
+++ b/rcc-ministry-catalog/src/main/resources/RCC Ministry Catalog.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="0" windowWidth="7860" windowHeight="8565"/>
+    <workbookView xWindow="46500" yWindow="0" windowWidth="7860" windowHeight="8565" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Outline" sheetId="5" r:id="rId1"/>
     <sheet name="Directory" sheetId="6" r:id="rId2"/>
     <sheet name="Dictionary" sheetId="7" r:id="rId3"/>
-    <sheet name="Audio Technician" sheetId="3" r:id="rId4"/>
+    <sheet name="Roles" sheetId="3" r:id="rId4"/>
     <sheet name="Reference" sheetId="2" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="245">
   <si>
     <t>Ministry Role:</t>
   </si>
@@ -263,12 +263,6 @@
     <t>1.1.1</t>
   </si>
   <si>
-    <t>Website Design</t>
-  </si>
-  <si>
-    <t>Website Maintenance</t>
-  </si>
-  <si>
     <t>1.1.2</t>
   </si>
   <si>
@@ -320,9 +314,6 @@
     <t>Tithe Counting</t>
   </si>
   <si>
-    <t>Building Committee</t>
-  </si>
-  <si>
     <t>Elizabeth Elder</t>
   </si>
   <si>
@@ -332,9 +323,6 @@
     <t>Capital Campaign</t>
   </si>
   <si>
-    <t>Property &amp; Building Maintenance</t>
-  </si>
-  <si>
     <t>Aesthetics Committee</t>
   </si>
   <si>
@@ -560,9 +548,6 @@
     <t>6.2.1</t>
   </si>
   <si>
-    <t>Home Group Leaders Meetings</t>
-  </si>
-  <si>
     <t>6.2.2</t>
   </si>
   <si>
@@ -731,9 +716,6 @@
     <t>Technology</t>
   </si>
   <si>
-    <t>1.1.3</t>
-  </si>
-  <si>
     <t>1.3.2</t>
   </si>
   <si>
@@ -747,6 +729,45 @@
   </si>
   <si>
     <t>Greeters</t>
+  </si>
+  <si>
+    <t>Ministry ID:</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>Facilities</t>
+  </si>
+  <si>
+    <t>1.4.3</t>
+  </si>
+  <si>
+    <t>1.4.4</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>1.6</t>
+  </si>
+  <si>
+    <t>Facility Maintenance</t>
+  </si>
+  <si>
+    <t>Robyn Richards</t>
+  </si>
+  <si>
+    <t>Desiree Yeago</t>
+  </si>
+  <si>
+    <t>Home Group Leader Training</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>Joanne Ward</t>
   </si>
 </sst>
 </file>
@@ -871,7 +892,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -921,7 +942,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -937,23 +957,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1022,10 +1040,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TDirectory" displayName="TDirectory" ref="A1:C14" totalsRowShown="0">
-  <autoFilter ref="A1:C14"/>
-  <sortState ref="A2:C13">
-    <sortCondition ref="A1:A13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TDirectory" displayName="TDirectory" ref="A1:C18" totalsRowShown="0">
+  <autoFilter ref="A1:C18"/>
+  <sortState ref="A2:C18">
+    <sortCondition ref="A1:A18"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" name="Name"/>
@@ -1334,12 +1352,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L79"/>
+  <dimension ref="A1:L78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
-      <selection pane="bottomLeft" activeCell="G46" sqref="G46:H46"/>
+      <selection pane="bottomLeft" activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1367,28 +1385,28 @@
         <v>72</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="I1" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>220</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1399,13 +1417,10 @@
         <v>74</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="F2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1413,10 +1428,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="D3" t="s">
-        <v>231</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>81</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1424,7 +1436,10 @@
         <v>75</v>
       </c>
       <c r="D4" t="s">
-        <v>76</v>
+        <v>233</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>87</v>
       </c>
       <c r="J4" t="s">
         <v>44</v>
@@ -1438,666 +1453,684 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C5" s="17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D5" t="s">
-        <v>77</v>
+        <v>82</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>197</v>
       </c>
       <c r="J5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="17">
+        <v>1.2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>81</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C7" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" t="s">
+        <v>84</v>
+      </c>
+      <c r="J7" t="s">
         <v>15</v>
-      </c>
-      <c r="K5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C6" s="17" t="s">
-        <v>232</v>
-      </c>
-      <c r="D6" t="s">
-        <v>84</v>
-      </c>
-      <c r="J6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="17">
-        <v>1.2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>83</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C8" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C10" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" t="s">
+        <v>91</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="J10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C9" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="D9" t="s">
-        <v>85</v>
-      </c>
-      <c r="J9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K9" t="s">
+      <c r="K10" t="s">
+        <v>18</v>
+      </c>
+      <c r="L10" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="17">
-        <v>1.3</v>
-      </c>
-      <c r="D10" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C11" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="D11" t="s">
         <v>92</v>
       </c>
-      <c r="D11" t="s">
-        <v>93</v>
-      </c>
       <c r="G11" s="16" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="J11" t="s">
         <v>15</v>
       </c>
       <c r="K11" t="s">
-        <v>18</v>
-      </c>
-      <c r="L11" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C12" s="17" t="s">
-        <v>233</v>
+      <c r="B12" s="17">
+        <v>1.4</v>
       </c>
       <c r="D12" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C13" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="G12" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="J12" t="s">
-        <v>15</v>
-      </c>
-      <c r="K12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="17">
-        <v>1.4</v>
-      </c>
       <c r="D13" t="s">
-        <v>226</v>
+        <v>95</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="J13" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C14" s="17" t="s">
-        <v>97</v>
+        <v>222</v>
       </c>
       <c r="D14" t="s">
-        <v>98</v>
+        <v>221</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>228</v>
-      </c>
-      <c r="J14" t="s">
-        <v>22</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C15" s="17" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="D15" t="s">
-        <v>95</v>
+        <v>239</v>
       </c>
       <c r="G15" s="16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C16" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="D16" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="17">
-        <v>1.5</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="J16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="D17" t="s">
+        <v>182</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="J17" t="s">
+        <v>20</v>
+      </c>
+      <c r="K17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="D18" t="s">
+        <v>183</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="17">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>97</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="17">
+        <v>2.1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>98</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C21" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="G16" s="16" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="17">
-        <v>1.6</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="D21" t="s">
         <v>100</v>
-      </c>
-      <c r="J17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="17">
-        <v>1.7</v>
-      </c>
-      <c r="D18" t="s">
-        <v>187</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="J18" t="s">
-        <v>20</v>
-      </c>
-      <c r="K18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="17">
-        <v>1.8</v>
-      </c>
-      <c r="D19" t="s">
-        <v>188</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="17">
-        <v>2</v>
-      </c>
-      <c r="D20" t="s">
-        <v>101</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="G20" s="16" t="s">
-        <v>199</v>
-      </c>
-      <c r="H20" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="17">
-        <v>2.1</v>
-      </c>
-      <c r="D21" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C22" s="17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D22" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C23" s="17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D23" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C24" s="17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D24" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C25" s="17" t="s">
-        <v>109</v>
+        <v>228</v>
       </c>
       <c r="D25" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C26" s="17" t="s">
-        <v>234</v>
+      <c r="B26" s="17">
+        <v>2.2000000000000002</v>
       </c>
       <c r="D26" t="s">
-        <v>114</v>
+        <v>107</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="17">
-        <v>2.2000000000000002</v>
+      <c r="C27" s="17" t="s">
+        <v>108</v>
       </c>
       <c r="D27" t="s">
-        <v>111</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>230</v>
+        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C28" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="D28" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="17">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D29" t="s">
+        <v>111</v>
+      </c>
+      <c r="G29" s="16" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C30" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="D28" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C29" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="D29" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="17">
-        <v>2.2999999999999998</v>
-      </c>
       <c r="D30" t="s">
-        <v>115</v>
+        <v>231</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C31" s="17" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D31" t="s">
-        <v>237</v>
+        <v>185</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C32" s="17" t="s">
-        <v>117</v>
+        <v>184</v>
       </c>
       <c r="D32" t="s">
-        <v>190</v>
+        <v>186</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C33" s="17" t="s">
-        <v>189</v>
+      <c r="B33" s="17">
+        <v>2.4</v>
       </c>
       <c r="D33" t="s">
-        <v>191</v>
-      </c>
-      <c r="E33" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G33" s="16" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C34" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="D34" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="17">
-        <v>2.4</v>
-      </c>
-      <c r="D34" t="s">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="17">
+        <v>3</v>
+      </c>
+      <c r="D35" t="s">
+        <v>115</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="17">
+        <v>3.1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>116</v>
+      </c>
+      <c r="G36" s="16" t="s">
         <v>118</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C35" s="17" t="s">
-        <v>235</v>
-      </c>
-      <c r="D35" t="s">
-        <v>236</v>
-      </c>
-      <c r="G35" s="16" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="17">
-        <v>3</v>
-      </c>
-      <c r="D36" t="s">
-        <v>119</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B37" s="17">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="D37" t="s">
+        <v>119</v>
+      </c>
+      <c r="G37" s="16" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C38" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="G37" s="16" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="17">
-        <v>3.2</v>
-      </c>
       <c r="D38" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C39" s="17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D39" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C40" s="17" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D40" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C41" s="17" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D41" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C42" s="17" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D42" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C43" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="D43" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="17">
+        <v>3.3</v>
+      </c>
+      <c r="D44" t="s">
         <v>132</v>
       </c>
-      <c r="D43" t="s">
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C45" s="17" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C44" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="D44" t="s">
+      <c r="D45" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="17">
-        <v>3.3</v>
-      </c>
-      <c r="D45" t="s">
-        <v>136</v>
+      <c r="G45" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="H45" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C46" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="D46" t="s">
+        <v>141</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B47" s="17">
+        <v>3.4</v>
+      </c>
+      <c r="D47" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C48" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="D46" t="s">
-        <v>139</v>
-      </c>
-      <c r="G46" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="H46" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C47" s="17" t="s">
+      <c r="D48" t="s">
         <v>138</v>
       </c>
-      <c r="D47" t="s">
-        <v>145</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B48" s="17">
-        <v>3.4</v>
-      </c>
-      <c r="D48" t="s">
-        <v>140</v>
+      <c r="G48" s="16" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C49" s="17" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D49" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="17">
+        <v>4</v>
+      </c>
+      <c r="D50" t="s">
+        <v>71</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="F50" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C50" s="17" t="s">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B51" s="17">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D51" t="s">
         <v>143</v>
       </c>
-      <c r="D50" t="s">
+      <c r="G51" s="16" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C52" s="17" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="17">
-        <v>4</v>
-      </c>
-      <c r="D51" t="s">
-        <v>71</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="F51" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B52" s="17">
-        <v>4.0999999999999996</v>
-      </c>
       <c r="D52" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C53" s="17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D53" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C54" s="17" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D54" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C55" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="D55" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B56" s="17">
+        <v>4.2</v>
+      </c>
+      <c r="D56" t="s">
         <v>152</v>
       </c>
-      <c r="D55" t="s">
+      <c r="G56" s="16" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C57" s="17" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C56" s="17" t="s">
+      <c r="D57" t="s">
         <v>154</v>
-      </c>
-      <c r="D56" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B57" s="17">
-        <v>4.2</v>
-      </c>
-      <c r="D57" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C58" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="D58" t="s">
+        <v>156</v>
+      </c>
+      <c r="J58" t="s">
+        <v>16</v>
+      </c>
+      <c r="K58" t="s">
+        <v>37</v>
+      </c>
+      <c r="L58" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="17">
+        <v>5</v>
+      </c>
+      <c r="D59" t="s">
         <v>157</v>
       </c>
-      <c r="D58" t="s">
+      <c r="E59" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="F59" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B60" s="17">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D60" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C61" s="17" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C59" s="17" t="s">
+      <c r="D61" t="s">
         <v>159</v>
       </c>
-      <c r="D59" t="s">
-        <v>160</v>
-      </c>
-      <c r="J59" t="s">
-        <v>16</v>
-      </c>
-      <c r="K59" t="s">
-        <v>37</v>
-      </c>
-      <c r="L59" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A60" s="17">
-        <v>5</v>
-      </c>
-      <c r="D60" t="s">
-        <v>161</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="F60" t="s">
-        <v>81</v>
-      </c>
-      <c r="G60" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="H60" t="s">
-        <v>201</v>
-      </c>
-      <c r="I60" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B61" s="17">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="D61" t="s">
+      <c r="G61" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="H61" t="s">
+        <v>196</v>
+      </c>
+      <c r="I61" t="s">
+        <v>197</v>
+      </c>
+      <c r="J61" t="s">
         <v>43</v>
+      </c>
+      <c r="K61" t="s">
+        <v>21</v>
+      </c>
+      <c r="L61" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C62" s="17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D62" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J62" t="s">
         <v>43</v>
       </c>
       <c r="K62" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="L62" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C63" s="17" t="s">
-        <v>164</v>
+        <v>188</v>
       </c>
       <c r="D63" t="s">
-        <v>165</v>
+        <v>187</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="G63" s="16" t="s">
+        <v>189</v>
       </c>
       <c r="J63" t="s">
         <v>43</v>
       </c>
       <c r="K63" t="s">
-        <v>35</v>
-      </c>
-      <c r="L63" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B64" s="17">
+        <v>5.2</v>
+      </c>
+      <c r="D64" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C65" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="D65" t="s">
+        <v>166</v>
+      </c>
+      <c r="J65" t="s">
+        <v>44</v>
+      </c>
+      <c r="K65" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C64" s="17" t="s">
-        <v>193</v>
-      </c>
-      <c r="D64" t="s">
-        <v>192</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="G64" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="J64" t="s">
+      <c r="L65" t="s">
         <v>43</v>
-      </c>
-      <c r="K64" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B65" s="17">
-        <v>5.2</v>
-      </c>
-      <c r="D65" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C66" s="17" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D66" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="J66" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="K66" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="L66" t="s">
         <v>43</v>
@@ -2105,10 +2138,10 @@
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C67" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="D67" t="s">
         <v>167</v>
-      </c>
-      <c r="D67" t="s">
-        <v>169</v>
       </c>
       <c r="J67" t="s">
         <v>15</v>
@@ -2121,182 +2154,168 @@
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C68" s="17" t="s">
+      <c r="A68" s="17">
+        <v>6</v>
+      </c>
+      <c r="D68" t="s">
+        <v>175</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B69" s="17">
+        <v>6.1</v>
+      </c>
+      <c r="D69" t="s">
         <v>168</v>
-      </c>
-      <c r="D68" t="s">
-        <v>171</v>
-      </c>
-      <c r="J68" t="s">
-        <v>15</v>
-      </c>
-      <c r="K68" t="s">
-        <v>42</v>
-      </c>
-      <c r="L68" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A69" s="17">
-        <v>6</v>
-      </c>
-      <c r="D69" t="s">
-        <v>180</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B70" s="17">
-        <v>6.1</v>
+        <v>6.2</v>
       </c>
       <c r="D70" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B71" s="17">
-        <v>6.2</v>
+      <c r="C71" s="17" t="s">
+        <v>170</v>
       </c>
       <c r="D71" t="s">
-        <v>173</v>
+        <v>242</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C72" s="17" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D72" t="s">
-        <v>175</v>
+        <v>172</v>
+      </c>
+      <c r="J72" t="s">
+        <v>20</v>
+      </c>
+      <c r="K72" t="s">
+        <v>31</v>
+      </c>
+      <c r="L72" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C73" s="17" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D73" t="s">
+        <v>174</v>
+      </c>
+      <c r="J73" t="s">
+        <v>15</v>
+      </c>
+      <c r="K73" t="s">
+        <v>34</v>
+      </c>
+      <c r="L73" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A74" s="17">
+        <v>7</v>
+      </c>
+      <c r="D74" t="s">
+        <v>32</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B75" s="17">
+        <v>7.1</v>
+      </c>
+      <c r="D75" t="s">
         <v>177</v>
       </c>
-      <c r="J73" t="s">
-        <v>20</v>
-      </c>
-      <c r="K73" t="s">
-        <v>31</v>
-      </c>
-      <c r="L73" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C74" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="D74" t="s">
+      <c r="G75" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="J74" t="s">
-        <v>15</v>
-      </c>
-      <c r="K74" t="s">
-        <v>34</v>
-      </c>
-      <c r="L74" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A75" s="17">
-        <v>7</v>
-      </c>
-      <c r="D75" t="s">
+      <c r="J75" t="s">
         <v>32</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="G75" s="16" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B76" s="17">
-        <v>7.1</v>
+        <v>7.2</v>
       </c>
       <c r="D76" t="s">
-        <v>182</v>
+        <v>178</v>
+      </c>
+      <c r="G76" s="16" t="s">
+        <v>244</v>
       </c>
       <c r="J76" t="s">
         <v>32</v>
       </c>
+      <c r="K76" t="s">
+        <v>41</v>
+      </c>
+      <c r="L76" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B77" s="17">
-        <v>7.2</v>
+        <v>7.3</v>
       </c>
       <c r="D77" t="s">
-        <v>183</v>
+        <v>190</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>225</v>
       </c>
       <c r="J77" t="s">
         <v>32</v>
       </c>
       <c r="K77" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L77" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B78" s="17">
-        <v>7.3</v>
+        <v>7.4</v>
       </c>
       <c r="D78" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="J78" t="s">
         <v>32</v>
       </c>
       <c r="K78" t="s">
+        <v>15</v>
+      </c>
+      <c r="L78" t="s">
         <v>35</v>
       </c>
-      <c r="L78" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B79" s="17">
-        <v>7.4</v>
-      </c>
-      <c r="D79" t="s">
-        <v>196</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="J79" t="s">
-        <v>32</v>
-      </c>
-      <c r="K79" t="s">
-        <v>15</v>
-      </c>
-      <c r="L79" t="s">
-        <v>35</v>
-      </c>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="3">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Not in directory" error="You have entered a person who is not in the Directory tab" sqref="G2:I9 H10:I27 G11:G27 I28:I200 G46:H200 G28:H44">
+  <dataValidations count="3">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Not in directory" error="You have entered a person who is not in the Directory tab" sqref="H9:I26 G10:G26 G2:I8 G27:H43 I27:I58 G45:H58 H60:I199 G75:G199 G60:G73">
       <formula1>INDIRECT("TDirectory[Name]")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E220">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E219">
       <formula1>INDIRECT("TMinistryTypes[Ministry Types]")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:L200">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:L199">
       <formula1>INDIRECT("TGifts[Gifts]")</formula1>
     </dataValidation>
   </dataValidations>
@@ -2307,10 +2326,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2322,130 +2341,159 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B5" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C5" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>215</v>
-      </c>
+        <v>241</v>
+      </c>
+      <c r="B6" s="20"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>202</v>
+        <v>93</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>206</v>
-      </c>
-      <c r="C7" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>82</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>213</v>
-      </c>
+        <v>195</v>
+      </c>
+      <c r="B8" s="20"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>201</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>209</v>
-      </c>
+        <v>244</v>
+      </c>
+      <c r="B9" s="20"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>218</v>
+        <v>201</v>
+      </c>
+      <c r="C10" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>228</v>
+        <v>80</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>81</v>
-      </c>
-      <c r="B12" t="s">
-        <v>210</v>
+        <v>223</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>122</v>
+        <v>196</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>146</v>
+        <v>194</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>214</v>
+        <v>213</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>240</v>
+      </c>
+      <c r="B15" s="20"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>118</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>142</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>243</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1"/>
+    <hyperlink ref="B10" r:id="rId1"/>
     <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="B9" r:id="rId3"/>
+    <hyperlink ref="B13" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2470,7 +2518,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C1" t="s">
         <v>46</v>
@@ -2478,7 +2526,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C2" t="s">
         <v>39</v>
@@ -2486,7 +2534,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C3" t="s">
         <v>44</v>
@@ -2544,7 +2592,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2643,10 +2691,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37:D37"/>
+      <selection activeCell="C32" sqref="C32:D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2663,508 +2711,504 @@
         <f>Reference!A1</f>
         <v>Ministry Role:</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="24"/>
+      <c r="D1" s="23"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="str">
+      <c r="A2" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="D2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="str">
         <f>Reference!A2</f>
         <v>Status:</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C3" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="str">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="str">
         <f>Reference!A3</f>
         <v>Filled by:</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C4" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="str">
-        <f>Reference!A5</f>
-        <v>In Ministry Area:</v>
-      </c>
-      <c r="C5" s="27" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D5" s="27"/>
+        <f>Reference!A7</f>
+        <v>For the benefit of:</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="14"/>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="str">
-        <f>Reference!A6</f>
-        <v>Under Ministry Role:</v>
-      </c>
-      <c r="C6" s="27" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="2"/>
+      <c r="A6" s="12"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="str">
-        <f>Reference!A7</f>
-        <v>For the benefit of:</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="str">
         <f>Reference!A9</f>
         <v>Position type:</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C7" s="6" t="s">
         <v>48</v>
       </c>
     </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="str">
+        <f>Reference!A10</f>
+        <v>Position open to:</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="25"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" ht="8.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="str">
-        <f>Reference!A10</f>
-        <v>Position open to:</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" ht="8.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="str">
         <f>Reference!A12</f>
         <v>Relevant gifts:</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C10" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="23"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="22"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="22"/>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="23"/>
+      <c r="C13" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="22"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="23"/>
+    <row r="14" spans="1:5" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="str">
+      <c r="A15" s="12" t="str">
         <f>Reference!A19</f>
         <v>Relevant skills:</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C15" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="23"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="C16" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="22"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="22"/>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="C18" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="23"/>
+      <c r="C18" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="22"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D19" s="23"/>
+    <row r="19" spans="1:5" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="23"/>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="1:5" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="str">
+      <c r="A20" s="12" t="str">
         <f>Reference!A25</f>
         <v>Personality:</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="C20" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="D22" s="23"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C21" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="22"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C22" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="22"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="D23" s="23"/>
+    <row r="23" spans="1:5" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="D24" s="23"/>
-      <c r="E24" s="2"/>
-    </row>
-    <row r="25" spans="1:5" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="str">
+      <c r="A24" s="12" t="str">
         <f>Reference!A31</f>
         <v>Length of service:</v>
       </c>
-      <c r="C26" s="22" t="s">
+      <c r="C24" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="D26" s="23"/>
-      <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="str">
+      <c r="D24" s="22"/>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="str">
         <f>Reference!A32</f>
         <v>Time commitments:</v>
       </c>
-      <c r="C27" s="22" t="s">
+      <c r="C25" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="D27" s="23"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C26" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="22"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C28" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="D28" s="23"/>
-      <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="1:5" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="2"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="str">
+      <c r="A28" s="12" t="str">
         <f>Reference!A38</f>
         <v>Responsibilities:</v>
       </c>
-      <c r="C30" s="22" t="s">
+      <c r="C28" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="D30" s="23"/>
-      <c r="E30" s="2"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C29" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29" s="22"/>
+      <c r="E29" s="5"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C30" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" s="22"/>
+      <c r="E30" s="5"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C31" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="D31" s="23"/>
+      <c r="C31" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" s="22"/>
       <c r="E31" s="5"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C32" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="D32" s="23"/>
+      <c r="C32" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" s="22"/>
       <c r="E32" s="5"/>
     </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C33" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="D33" s="23"/>
-      <c r="E33" s="5"/>
-    </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C34" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="D34" s="23"/>
-      <c r="E34" s="5"/>
-    </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-    </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
-    </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-    </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
-    </row>
-    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
-    </row>
-    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
-    </row>
-    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C41" s="21"/>
-      <c r="D41" s="21"/>
-    </row>
-    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-    </row>
-    <row r="43" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C43" s="21"/>
-      <c r="D43" s="21"/>
-    </row>
-    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
-    </row>
-    <row r="45" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C45" s="21"/>
-      <c r="D45" s="21"/>
-    </row>
-    <row r="46" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
-    </row>
-    <row r="47" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
-    </row>
-    <row r="48" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C48" s="21"/>
-      <c r="D48" s="21"/>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+    </row>
+    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+    </row>
+    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+    </row>
+    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+    </row>
+    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C44" s="26"/>
+      <c r="D44" s="26"/>
+    </row>
+    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C45" s="26"/>
+      <c r="D45" s="26"/>
+    </row>
+    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
+    </row>
+    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
+    </row>
+    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C48" s="26"/>
+      <c r="D48" s="26"/>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C49" s="21"/>
-      <c r="D49" s="21"/>
+      <c r="C49" s="26"/>
+      <c r="D49" s="26"/>
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
+      <c r="C50" s="26"/>
+      <c r="D50" s="26"/>
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C51" s="21"/>
-      <c r="D51" s="21"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="26"/>
     </row>
     <row r="52" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
+      <c r="C52" s="26"/>
+      <c r="D52" s="26"/>
     </row>
     <row r="53" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C53" s="21"/>
-      <c r="D53" s="21"/>
+      <c r="C53" s="26"/>
+      <c r="D53" s="26"/>
     </row>
     <row r="54" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C54" s="21"/>
-      <c r="D54" s="21"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="26"/>
     </row>
     <row r="55" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C55" s="21"/>
-      <c r="D55" s="21"/>
+      <c r="C55" s="26"/>
+      <c r="D55" s="26"/>
     </row>
     <row r="56" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C56" s="21"/>
-      <c r="D56" s="21"/>
+      <c r="C56" s="26"/>
+      <c r="D56" s="26"/>
     </row>
     <row r="57" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C57" s="21"/>
-      <c r="D57" s="21"/>
+      <c r="C57" s="26"/>
+      <c r="D57" s="26"/>
     </row>
     <row r="58" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C58" s="21"/>
-      <c r="D58" s="21"/>
+      <c r="C58" s="26"/>
+      <c r="D58" s="26"/>
     </row>
     <row r="59" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C59" s="21"/>
-      <c r="D59" s="21"/>
+      <c r="C59" s="26"/>
+      <c r="D59" s="26"/>
     </row>
     <row r="60" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C60" s="21"/>
-      <c r="D60" s="21"/>
+      <c r="C60" s="26"/>
+      <c r="D60" s="26"/>
     </row>
     <row r="61" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C61" s="21"/>
-      <c r="D61" s="21"/>
+      <c r="C61" s="26"/>
+      <c r="D61" s="26"/>
     </row>
     <row r="62" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C62" s="21"/>
-      <c r="D62" s="21"/>
+      <c r="C62" s="26"/>
+      <c r="D62" s="26"/>
     </row>
     <row r="63" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C63" s="21"/>
-      <c r="D63" s="21"/>
+      <c r="C63" s="26"/>
+      <c r="D63" s="26"/>
     </row>
     <row r="64" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C64" s="21"/>
-      <c r="D64" s="21"/>
+      <c r="C64" s="26"/>
+      <c r="D64" s="26"/>
     </row>
     <row r="65" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C65" s="21"/>
-      <c r="D65" s="21"/>
+      <c r="C65" s="26"/>
+      <c r="D65" s="26"/>
     </row>
     <row r="66" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C66" s="21"/>
-      <c r="D66" s="21"/>
+      <c r="C66" s="26"/>
+      <c r="D66" s="26"/>
     </row>
     <row r="67" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C67" s="21"/>
-      <c r="D67" s="21"/>
+      <c r="C67" s="26"/>
+      <c r="D67" s="26"/>
     </row>
     <row r="68" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C68" s="21"/>
-      <c r="D68" s="21"/>
+      <c r="C68" s="26"/>
+      <c r="D68" s="26"/>
     </row>
     <row r="69" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C69" s="21"/>
-      <c r="D69" s="21"/>
+      <c r="C69" s="26"/>
+      <c r="D69" s="26"/>
     </row>
     <row r="70" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C70" s="21"/>
-      <c r="D70" s="21"/>
+      <c r="C70" s="26"/>
+      <c r="D70" s="26"/>
     </row>
     <row r="71" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C71" s="21"/>
-      <c r="D71" s="21"/>
+      <c r="C71" s="26"/>
+      <c r="D71" s="26"/>
     </row>
     <row r="72" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C72" s="21"/>
-      <c r="D72" s="21"/>
+      <c r="C72" s="26"/>
+      <c r="D72" s="26"/>
     </row>
     <row r="73" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C73" s="21"/>
-      <c r="D73" s="21"/>
+      <c r="C73" s="26"/>
+      <c r="D73" s="26"/>
     </row>
     <row r="74" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C74" s="21"/>
-      <c r="D74" s="21"/>
+      <c r="C74" s="26"/>
+      <c r="D74" s="26"/>
     </row>
     <row r="75" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C75" s="21"/>
-      <c r="D75" s="21"/>
+      <c r="C75" s="26"/>
+      <c r="D75" s="26"/>
     </row>
     <row r="76" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C76" s="21"/>
-      <c r="D76" s="21"/>
+      <c r="C76" s="26"/>
+      <c r="D76" s="26"/>
     </row>
     <row r="77" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C77" s="21"/>
-      <c r="D77" s="21"/>
+      <c r="C77" s="26"/>
+      <c r="D77" s="26"/>
     </row>
     <row r="78" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C78" s="21"/>
-      <c r="D78" s="21"/>
+      <c r="C78" s="26"/>
+      <c r="D78" s="26"/>
     </row>
     <row r="79" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C79" s="21"/>
-      <c r="D79" s="21"/>
+      <c r="C79" s="26"/>
+      <c r="D79" s="26"/>
     </row>
     <row r="80" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C80" s="21"/>
-      <c r="D80" s="21"/>
+      <c r="C80" s="26"/>
+      <c r="D80" s="26"/>
     </row>
     <row r="81" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C81" s="21"/>
-      <c r="D81" s="21"/>
+      <c r="C81" s="26"/>
+      <c r="D81" s="26"/>
     </row>
     <row r="82" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C82" s="21"/>
-      <c r="D82" s="21"/>
+      <c r="C82" s="26"/>
+      <c r="D82" s="26"/>
     </row>
     <row r="83" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C83" s="21"/>
-      <c r="D83" s="21"/>
-    </row>
-    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C84" s="21"/>
-      <c r="D84" s="21"/>
-    </row>
-    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C85" s="21"/>
-      <c r="D85" s="21"/>
+      <c r="C83" s="26"/>
+      <c r="D83" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="75">
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
+  <mergeCells count="73">
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C47:D47"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C49:D49"/>
     <mergeCell ref="C38:D38"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="C40:D40"/>
@@ -3174,46 +3218,33 @@
     <mergeCell ref="C44:D44"/>
     <mergeCell ref="C45:D45"/>
     <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C11:D11"/>
   </mergeCells>
-  <conditionalFormatting sqref="C2">
+  <conditionalFormatting sqref="C3">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"Filled"</formula>
     </cfRule>
@@ -3225,23 +3256,19 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3">
       <formula1>INDIRECT("Reference!StatusList")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7">
       <formula1>INDIRECT("Reference!PosTypeList")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12:D15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10:D13">
       <formula1>INDIRECT("Reference!GiftList")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E12:E16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E10:E14">
       <formula1>GiftList</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="C6:D6" location="'Media Ministry Head'!C1" display="'Media Ministry Head'!C1"/>
-    <hyperlink ref="C5:D5" location="Overview!S2" display="Overview!S2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3271,8 +3298,8 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
       <c r="E1" s="1"/>
       <c r="F1" t="s">
         <v>45</v>
@@ -3305,8 +3332,8 @@
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="29"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="28"/>
       <c r="E3" s="2"/>
       <c r="F3" t="s">
         <v>2</v>
@@ -3331,8 +3358,8 @@
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
       <c r="E5" s="2"/>
       <c r="G5" t="s">
         <v>29</v>
@@ -3342,8 +3369,8 @@
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
       <c r="E6" s="2"/>
       <c r="G6" t="s">
         <v>23</v>
@@ -3381,8 +3408,8 @@
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="29"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="28"/>
       <c r="E10" s="2"/>
       <c r="G10" t="s">
         <v>22</v>
@@ -3398,8 +3425,8 @@
       <c r="A12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="29"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28"/>
       <c r="E12" s="2"/>
       <c r="G12" t="s">
         <v>30</v>
@@ -3407,8 +3434,8 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="29"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="28"/>
       <c r="E13" s="2"/>
       <c r="G13" t="s">
         <v>31</v>
@@ -3416,8 +3443,8 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="29"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="28"/>
       <c r="E14" s="2"/>
       <c r="G14" t="s">
         <v>33</v>
@@ -3425,8 +3452,8 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="29"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="28"/>
       <c r="E15" s="2"/>
       <c r="G15" t="s">
         <v>34</v>
@@ -3434,8 +3461,8 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="29"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="28"/>
       <c r="E16" s="2"/>
       <c r="G16" t="s">
         <v>35</v>
@@ -3463,8 +3490,8 @@
       <c r="A19" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="28"/>
-      <c r="D19" s="29"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="28"/>
       <c r="E19" s="2"/>
       <c r="G19" t="s">
         <v>16</v>
@@ -3472,8 +3499,8 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="29"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="28"/>
       <c r="E20" s="2"/>
       <c r="G20" t="s">
         <v>43</v>
@@ -3481,8 +3508,8 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="29"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="28"/>
       <c r="E21" s="2"/>
       <c r="G21" t="s">
         <v>15</v>
@@ -3490,8 +3517,8 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="29"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="28"/>
       <c r="E22" s="2"/>
       <c r="G22" t="s">
         <v>32</v>
@@ -3499,8 +3526,8 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="29"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="28"/>
       <c r="E23" s="2"/>
       <c r="G23" t="s">
         <v>41</v>
@@ -3519,8 +3546,8 @@
       <c r="A25" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C25" s="28"/>
-      <c r="D25" s="29"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="28"/>
       <c r="E25" s="2"/>
       <c r="G25" t="s">
         <v>40</v>
@@ -3528,8 +3555,8 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="29"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="28"/>
       <c r="E26" s="2"/>
       <c r="G26" t="s">
         <v>17</v>
@@ -3537,8 +3564,8 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="29"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="28"/>
       <c r="E27" s="2"/>
       <c r="G27" t="s">
         <v>36</v>
@@ -3546,8 +3573,8 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="29"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="28"/>
       <c r="E28" s="2"/>
       <c r="G28" t="s">
         <v>25</v>
@@ -3555,8 +3582,8 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="29"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="28"/>
       <c r="E29" s="2"/>
       <c r="G29" t="s">
         <v>26</v>
@@ -3575,8 +3602,8 @@
       <c r="A31" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C31" s="28"/>
-      <c r="D31" s="29"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="28"/>
       <c r="E31" s="2"/>
       <c r="G31" t="s">
         <v>27</v>
@@ -3586,32 +3613,32 @@
       <c r="A32" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="28"/>
-      <c r="D32" s="29"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="28"/>
       <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="29"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="28"/>
       <c r="E33" s="2"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="29"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="28"/>
       <c r="E34" s="2"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
-      <c r="C35" s="28"/>
-      <c r="D35" s="29"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="28"/>
       <c r="E35" s="2"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
-      <c r="C36" s="28"/>
-      <c r="D36" s="29"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="28"/>
       <c r="E36" s="2"/>
     </row>
     <row r="37" spans="1:5" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -3624,315 +3651,247 @@
       <c r="A38" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="28"/>
-      <c r="D38" s="29"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="28"/>
       <c r="E38" s="2"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="31"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="32"/>
       <c r="E39" s="5"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C40" s="30"/>
-      <c r="D40" s="31"/>
+      <c r="C40" s="31"/>
+      <c r="D40" s="32"/>
       <c r="E40" s="5"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C41" s="30"/>
-      <c r="D41" s="31"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="32"/>
       <c r="E41" s="5"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C42" s="30"/>
-      <c r="D42" s="31"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="32"/>
       <c r="E42" s="5"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C43" s="30"/>
-      <c r="D43" s="31"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="32"/>
       <c r="E43" s="5"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C44" s="30"/>
-      <c r="D44" s="31"/>
+      <c r="C44" s="31"/>
+      <c r="D44" s="32"/>
       <c r="E44" s="5"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C45" s="21"/>
-      <c r="D45" s="21"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="26"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C48" s="21"/>
-      <c r="D48" s="21"/>
+      <c r="C48" s="26"/>
+      <c r="D48" s="26"/>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C49" s="21"/>
-      <c r="D49" s="21"/>
+      <c r="C49" s="26"/>
+      <c r="D49" s="26"/>
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
+      <c r="C50" s="26"/>
+      <c r="D50" s="26"/>
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C51" s="21"/>
-      <c r="D51" s="21"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="26"/>
     </row>
     <row r="52" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
+      <c r="C52" s="26"/>
+      <c r="D52" s="26"/>
     </row>
     <row r="53" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C53" s="21"/>
-      <c r="D53" s="21"/>
+      <c r="C53" s="26"/>
+      <c r="D53" s="26"/>
     </row>
     <row r="54" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C54" s="21"/>
-      <c r="D54" s="21"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="26"/>
     </row>
     <row r="55" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C55" s="21"/>
-      <c r="D55" s="21"/>
+      <c r="C55" s="26"/>
+      <c r="D55" s="26"/>
     </row>
     <row r="56" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C56" s="21"/>
-      <c r="D56" s="21"/>
+      <c r="C56" s="26"/>
+      <c r="D56" s="26"/>
     </row>
     <row r="57" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C57" s="21"/>
-      <c r="D57" s="21"/>
+      <c r="C57" s="26"/>
+      <c r="D57" s="26"/>
     </row>
     <row r="58" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C58" s="21"/>
-      <c r="D58" s="21"/>
+      <c r="C58" s="26"/>
+      <c r="D58" s="26"/>
     </row>
     <row r="59" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C59" s="21"/>
-      <c r="D59" s="21"/>
+      <c r="C59" s="26"/>
+      <c r="D59" s="26"/>
     </row>
     <row r="60" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C60" s="21"/>
-      <c r="D60" s="21"/>
+      <c r="C60" s="26"/>
+      <c r="D60" s="26"/>
     </row>
     <row r="61" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C61" s="21"/>
-      <c r="D61" s="21"/>
+      <c r="C61" s="26"/>
+      <c r="D61" s="26"/>
     </row>
     <row r="62" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C62" s="21"/>
-      <c r="D62" s="21"/>
+      <c r="C62" s="26"/>
+      <c r="D62" s="26"/>
     </row>
     <row r="63" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C63" s="21"/>
-      <c r="D63" s="21"/>
+      <c r="C63" s="26"/>
+      <c r="D63" s="26"/>
     </row>
     <row r="64" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C64" s="21"/>
-      <c r="D64" s="21"/>
+      <c r="C64" s="26"/>
+      <c r="D64" s="26"/>
     </row>
     <row r="65" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C65" s="21"/>
-      <c r="D65" s="21"/>
+      <c r="C65" s="26"/>
+      <c r="D65" s="26"/>
     </row>
     <row r="66" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C66" s="21"/>
-      <c r="D66" s="21"/>
+      <c r="C66" s="26"/>
+      <c r="D66" s="26"/>
     </row>
     <row r="67" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C67" s="21"/>
-      <c r="D67" s="21"/>
+      <c r="C67" s="26"/>
+      <c r="D67" s="26"/>
     </row>
     <row r="68" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C68" s="21"/>
-      <c r="D68" s="21"/>
+      <c r="C68" s="26"/>
+      <c r="D68" s="26"/>
     </row>
     <row r="69" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C69" s="21"/>
-      <c r="D69" s="21"/>
+      <c r="C69" s="26"/>
+      <c r="D69" s="26"/>
     </row>
     <row r="70" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C70" s="21"/>
-      <c r="D70" s="21"/>
+      <c r="C70" s="26"/>
+      <c r="D70" s="26"/>
     </row>
     <row r="71" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C71" s="21"/>
-      <c r="D71" s="21"/>
+      <c r="C71" s="26"/>
+      <c r="D71" s="26"/>
     </row>
     <row r="72" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C72" s="21"/>
-      <c r="D72" s="21"/>
+      <c r="C72" s="26"/>
+      <c r="D72" s="26"/>
     </row>
     <row r="73" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C73" s="21"/>
-      <c r="D73" s="21"/>
+      <c r="C73" s="26"/>
+      <c r="D73" s="26"/>
     </row>
     <row r="74" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C74" s="21"/>
-      <c r="D74" s="21"/>
+      <c r="C74" s="26"/>
+      <c r="D74" s="26"/>
     </row>
     <row r="75" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C75" s="21"/>
-      <c r="D75" s="21"/>
+      <c r="C75" s="26"/>
+      <c r="D75" s="26"/>
     </row>
     <row r="76" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C76" s="21"/>
-      <c r="D76" s="21"/>
+      <c r="C76" s="26"/>
+      <c r="D76" s="26"/>
     </row>
     <row r="77" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C77" s="21"/>
-      <c r="D77" s="21"/>
+      <c r="C77" s="26"/>
+      <c r="D77" s="26"/>
     </row>
     <row r="78" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C78" s="21"/>
-      <c r="D78" s="21"/>
+      <c r="C78" s="26"/>
+      <c r="D78" s="26"/>
     </row>
     <row r="79" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C79" s="21"/>
-      <c r="D79" s="21"/>
+      <c r="C79" s="26"/>
+      <c r="D79" s="26"/>
     </row>
     <row r="80" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C80" s="21"/>
-      <c r="D80" s="21"/>
+      <c r="C80" s="26"/>
+      <c r="D80" s="26"/>
     </row>
     <row r="81" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C81" s="21"/>
-      <c r="D81" s="21"/>
+      <c r="C81" s="26"/>
+      <c r="D81" s="26"/>
     </row>
     <row r="82" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C82" s="21"/>
-      <c r="D82" s="21"/>
+      <c r="C82" s="26"/>
+      <c r="D82" s="26"/>
     </row>
     <row r="83" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C83" s="21"/>
-      <c r="D83" s="21"/>
+      <c r="C83" s="26"/>
+      <c r="D83" s="26"/>
     </row>
     <row r="84" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C84" s="21"/>
-      <c r="D84" s="21"/>
+      <c r="C84" s="26"/>
+      <c r="D84" s="26"/>
     </row>
     <row r="85" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C85" s="21"/>
-      <c r="D85" s="21"/>
+      <c r="C85" s="26"/>
+      <c r="D85" s="26"/>
     </row>
     <row r="86" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C86" s="21"/>
-      <c r="D86" s="21"/>
+      <c r="C86" s="26"/>
+      <c r="D86" s="26"/>
     </row>
     <row r="87" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C87" s="21"/>
-      <c r="D87" s="21"/>
+      <c r="C87" s="26"/>
+      <c r="D87" s="26"/>
     </row>
     <row r="88" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C88" s="21"/>
-      <c r="D88" s="21"/>
+      <c r="C88" s="26"/>
+      <c r="D88" s="26"/>
     </row>
     <row r="89" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C89" s="21"/>
-      <c r="D89" s="21"/>
+      <c r="C89" s="26"/>
+      <c r="D89" s="26"/>
     </row>
     <row r="90" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C90" s="21"/>
-      <c r="D90" s="21"/>
+      <c r="C90" s="26"/>
+      <c r="D90" s="26"/>
     </row>
     <row r="91" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C91" s="21"/>
-      <c r="D91" s="21"/>
+      <c r="C91" s="26"/>
+      <c r="D91" s="26"/>
     </row>
     <row r="92" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C92" s="21"/>
-      <c r="D92" s="21"/>
+      <c r="C92" s="26"/>
+      <c r="D92" s="26"/>
     </row>
     <row r="93" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C93" s="21"/>
-      <c r="D93" s="21"/>
+      <c r="C93" s="26"/>
+      <c r="D93" s="26"/>
     </row>
     <row r="94" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C94" s="21"/>
-      <c r="D94" s="21"/>
+      <c r="C94" s="26"/>
+      <c r="D94" s="26"/>
     </row>
     <row r="95" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C95" s="21"/>
-      <c r="D95" s="21"/>
+      <c r="C95" s="26"/>
+      <c r="D95" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="84">
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C81:D81"/>
     <mergeCell ref="C94:D94"/>
     <mergeCell ref="C95:D95"/>
     <mergeCell ref="C10:D10"/>
@@ -3949,6 +3908,74 @@
     <mergeCell ref="C86:D86"/>
     <mergeCell ref="C87:D87"/>
     <mergeCell ref="C76:D76"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
   </mergeCells>
   <conditionalFormatting sqref="C2">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">

</xml_diff>